<commit_message>
ageStdDev running time updated
ageStdDev running time [pseudo-DP, 2M2R] updated

readme.md updated
</commit_message>
<xml_diff>
--- a/doc/MR_RunningTime.xlsx
+++ b/doc/MR_RunningTime.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yoonseung/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yoonseung/Desktop/MapReduce/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="980" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4800" yWindow="980" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="1.NumericalSummarization" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,46 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="P6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>stackoverflow.com users' data (1G)
+Pseudo-DP:
+‘14 MacBook Pro, 2.8 GHz Intel Core i5    8GB 1600 MHz DDR3, 500GB SSD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>stackoverflow.com users' data (1G)
+Pseudo-DP:
+‘14 MacBook Pro, 2.8 GHz Intel Core i5    8GB 1600 MHz DDR3, 500GB SSD</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -76,9 +116,6 @@
     <t>Avg</t>
   </si>
   <si>
-    <t>Average of user's age</t>
-  </si>
-  <si>
     <t>Min/Max Count</t>
   </si>
   <si>
@@ -99,9 +136,6 @@
     <t>Fully-DP: RaspberryPi Cluster (3-node)</t>
   </si>
   <si>
-    <t>Median and standard deviation</t>
-  </si>
-  <si>
     <t>Distributed grep</t>
   </si>
   <si>
@@ -119,12 +153,18 @@
   <si>
     <t>io.sort.mb variation</t>
   </si>
+  <si>
+    <t>Average of users' age</t>
+  </si>
+  <si>
+    <t>Standard deviation of users' age</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -169,6 +209,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="6">
@@ -235,7 +281,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -254,17 +300,23 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -273,11 +325,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -556,29 +608,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="12"/>
     </row>
@@ -586,90 +638,90 @@
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17" t="s">
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="10" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="14" t="s">
         <v>2</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="10" t="s">
+      <c r="H7" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="14" t="s">
         <v>2</v>
       </c>
       <c r="K7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="M7" s="10" t="s">
+      <c r="L7" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="N7" s="14" t="s">
         <v>2</v>
       </c>
       <c r="O7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="P7" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="10" t="s">
+      <c r="P7" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="R7" s="10" t="s">
+      <c r="R7" s="14" t="s">
         <v>2</v>
       </c>
       <c r="S7" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="16" t="s">
-        <v>16</v>
+    <row r="8" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
@@ -690,14 +742,17 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="3"/>
+      <c r="O8" s="23"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="3"/>
+      <c r="S8" s="23">
+        <f t="shared" ref="S8:S10" si="0">SUM(P8:R8)/3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="15"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
@@ -711,20 +766,23 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="13">
-        <f t="shared" ref="K9:K32" si="0">H9</f>
+        <f t="shared" ref="K9:K32" si="1">H9</f>
         <v>87</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="3"/>
+      <c r="O9" s="23"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="3"/>
+      <c r="S9" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="15"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -738,20 +796,23 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="3"/>
+      <c r="O10" s="23"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="3"/>
+      <c r="S10" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="15"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
@@ -765,20 +826,23 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="3"/>
+      <c r="O11" s="23"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="3"/>
+      <c r="S11" s="23">
+        <f>SUM(P11:R11)/3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="21"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
@@ -791,21 +855,24 @@
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="13">
-        <f t="shared" si="0"/>
+      <c r="K12" s="24">
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
-      <c r="O12" s="6"/>
+      <c r="O12" s="23"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
-      <c r="S12" s="6"/>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B13" s="14" t="s">
+      <c r="S12" s="23">
+        <f>SUM(P12:R12)/3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -821,20 +888,29 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>199</v>
       </c>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="9"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="8">
+        <v>220</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>197</v>
+      </c>
+      <c r="R13" s="8">
+        <v>195</v>
+      </c>
+      <c r="S13" s="23">
+        <f t="shared" ref="S13:S15" si="2">SUM(P13:R13)/3</f>
+        <v>204</v>
+      </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B14" s="15"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
@@ -848,20 +924,29 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>112</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="3"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="2">
+        <v>116</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>115</v>
+      </c>
+      <c r="R14" s="2">
+        <v>121</v>
+      </c>
+      <c r="S14" s="23">
+        <f t="shared" si="2"/>
+        <v>117.33333333333333</v>
+      </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="15"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
@@ -875,20 +960,29 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="3"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="2">
+        <v>85</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>88</v>
+      </c>
+      <c r="R15" s="2">
+        <v>86</v>
+      </c>
+      <c r="S15" s="23">
+        <f t="shared" si="2"/>
+        <v>86.333333333333329</v>
+      </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B16" s="15"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
@@ -902,20 +996,29 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="3"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="2">
+        <v>61</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>68</v>
+      </c>
+      <c r="R16" s="2">
+        <v>65</v>
+      </c>
+      <c r="S16" s="23">
+        <f>SUM(P16:R16)/3</f>
+        <v>64.666666666666671</v>
+      </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B17" s="21"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
@@ -928,21 +1031,30 @@
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="13">
-        <f t="shared" si="0"/>
+      <c r="K17" s="24">
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="6"/>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B18" s="14" t="s">
+      <c r="O17" s="23"/>
+      <c r="P17" s="5">
+        <v>57</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>59</v>
+      </c>
+      <c r="R17" s="5">
+        <v>53</v>
+      </c>
+      <c r="S17" s="23">
+        <f>SUM(P17:R17)/3</f>
+        <v>56.333333333333336</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -956,20 +1068,23 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
-      <c r="O18" s="9"/>
+      <c r="O18" s="23"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
-      <c r="S18" s="9"/>
+      <c r="S18" s="23">
+        <f t="shared" ref="S18:S20" si="3">SUM(P18:R18)/3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B19" s="15"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
@@ -981,20 +1096,23 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
-      <c r="O19" s="3"/>
+      <c r="O19" s="23"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
-      <c r="S19" s="3"/>
+      <c r="S19" s="23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B20" s="15"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
@@ -1006,20 +1124,23 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
-      <c r="O20" s="3"/>
+      <c r="O20" s="23"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
-      <c r="S20" s="3"/>
+      <c r="S20" s="23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B21" s="15"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
@@ -1031,20 +1152,23 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
-      <c r="O21" s="3"/>
+      <c r="O21" s="23"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
-      <c r="S21" s="3"/>
+      <c r="S21" s="23">
+        <f>SUM(P21:R21)/3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B22" s="21"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="4" t="s">
         <v>7</v>
       </c>
@@ -1055,21 +1179,24 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="13">
-        <f t="shared" si="0"/>
+      <c r="K22" s="24">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
-      <c r="O22" s="6"/>
+      <c r="O22" s="23"/>
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
-      <c r="S22" s="6"/>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B23" s="14" t="s">
+      <c r="S22" s="23">
+        <f>SUM(P22:R22)/3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -1083,20 +1210,23 @@
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
-      <c r="O23" s="9"/>
+      <c r="O23" s="23"/>
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
-      <c r="S23" s="9"/>
+      <c r="S23" s="23">
+        <f t="shared" ref="S23:S25" si="4">SUM(P23:R23)/3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B24" s="15"/>
+      <c r="B24" s="18"/>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1110,20 +1240,23 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>375</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
-      <c r="O24" s="3"/>
+      <c r="O24" s="23"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
-      <c r="S24" s="3"/>
+      <c r="S24" s="23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B25" s="15"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
@@ -1137,20 +1270,23 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>396</v>
       </c>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
-      <c r="O25" s="3"/>
+      <c r="O25" s="23"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
-      <c r="S25" s="3"/>
+      <c r="S25" s="23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B26" s="15"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
@@ -1164,20 +1300,23 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>442</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="3"/>
+      <c r="O26" s="23"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
-      <c r="S26" s="3"/>
+      <c r="S26" s="23">
+        <f>SUM(P26:R26)/3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B27" s="21"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="4" t="s">
         <v>7</v>
       </c>
@@ -1190,21 +1329,24 @@
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="13">
-        <f t="shared" si="0"/>
+      <c r="K27" s="24">
+        <f t="shared" si="1"/>
         <v>548</v>
       </c>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="6"/>
+      <c r="O27" s="23"/>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
-      <c r="S27" s="6"/>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B28" s="14" t="s">
+      <c r="S27" s="23">
+        <f>SUM(P27:R27)/3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -1218,20 +1360,23 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
-      <c r="O28" s="9"/>
+      <c r="O28" s="23"/>
       <c r="P28" s="8"/>
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
-      <c r="S28" s="9"/>
+      <c r="S28" s="23">
+        <f t="shared" ref="S28:S30" si="5">SUM(P28:R28)/3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B29" s="16"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
@@ -1245,20 +1390,23 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>313</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="3"/>
+      <c r="O29" s="23"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
-      <c r="S29" s="3"/>
+      <c r="S29" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B30" s="16"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="1" t="s">
         <v>5</v>
       </c>
@@ -1272,20 +1420,23 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>296</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="O30" s="3"/>
+      <c r="O30" s="23"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
-      <c r="S30" s="3"/>
+      <c r="S30" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B31" s="16"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="1" t="s">
         <v>6</v>
       </c>
@@ -1299,20 +1450,23 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>350</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="O31" s="3"/>
+      <c r="O31" s="23"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
-      <c r="S31" s="3"/>
+      <c r="S31" s="23">
+        <f>SUM(P31:R31)/3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B32" s="20"/>
+      <c r="B32" s="19"/>
       <c r="C32" s="4" t="s">
         <v>7</v>
       </c>
@@ -1325,95 +1479,98 @@
       </c>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
-      <c r="K32" s="13">
-        <f t="shared" si="0"/>
+      <c r="K32" s="24">
+        <f t="shared" si="1"/>
         <v>557</v>
       </c>
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
-      <c r="O32" s="6"/>
+      <c r="O32" s="25"/>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
-      <c r="S32" s="6"/>
+      <c r="S32" s="25">
+        <f>SUM(P32:R32)/3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="20"/>
+      <c r="D34" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="17"/>
-      <c r="P34" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q34" s="17"/>
-      <c r="R34" s="17"/>
-      <c r="S34" s="17"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="15"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E35" s="10" t="s">
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="14" t="s">
         <v>2</v>
       </c>
       <c r="G35" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I35" s="10" t="s">
+      <c r="H35" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I35" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J35" s="10" t="s">
+      <c r="J35" s="14" t="s">
         <v>2</v>
       </c>
       <c r="K35" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L35" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="M35" s="10" t="s">
+      <c r="L35" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M35" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N35" s="10" t="s">
+      <c r="N35" s="14" t="s">
         <v>2</v>
       </c>
       <c r="O35" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="P35" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="10" t="s">
+      <c r="P35" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="R35" s="10" t="s">
+      <c r="R35" s="14" t="s">
         <v>2</v>
       </c>
       <c r="S35" s="11" t="s">
@@ -1421,8 +1578,8 @@
       </c>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B36" s="16" t="s">
-        <v>16</v>
+      <c r="B36" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>3</v>
@@ -1445,7 +1602,7 @@
       <c r="S36" s="3"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B37" s="16"/>
+      <c r="B37" s="17"/>
       <c r="C37" s="1" t="s">
         <v>4</v>
       </c>
@@ -1467,7 +1624,7 @@
       <c r="S37" s="3"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B38" s="15"/>
+      <c r="B38" s="18"/>
       <c r="C38" s="1" t="s">
         <v>5</v>
       </c>
@@ -1489,7 +1646,7 @@
       <c r="S38" s="3"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B39" s="15"/>
+      <c r="B39" s="18"/>
       <c r="C39" s="4" t="s">
         <v>6</v>
       </c>
@@ -1511,7 +1668,7 @@
       <c r="S39" s="3"/>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1535,7 +1692,7 @@
       <c r="S40" s="9"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B41" s="16"/>
+      <c r="B41" s="17"/>
       <c r="C41" s="1" t="s">
         <v>4</v>
       </c>
@@ -1557,7 +1714,7 @@
       <c r="S41" s="3"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B42" s="15"/>
+      <c r="B42" s="18"/>
       <c r="C42" s="1" t="s">
         <v>5</v>
       </c>
@@ -1579,7 +1736,7 @@
       <c r="S42" s="3"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B43" s="15"/>
+      <c r="B43" s="18"/>
       <c r="C43" s="4" t="s">
         <v>6</v>
       </c>
@@ -1601,7 +1758,7 @@
       <c r="S43" s="3"/>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1625,7 +1782,7 @@
       <c r="S44" s="9"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B45" s="16"/>
+      <c r="B45" s="17"/>
       <c r="C45" s="1" t="s">
         <v>4</v>
       </c>
@@ -1647,7 +1804,7 @@
       <c r="S45" s="3"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B46" s="15"/>
+      <c r="B46" s="18"/>
       <c r="C46" s="1" t="s">
         <v>5</v>
       </c>
@@ -1669,7 +1826,7 @@
       <c r="S46" s="3"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B47" s="15"/>
+      <c r="B47" s="18"/>
       <c r="C47" s="4" t="s">
         <v>6</v>
       </c>
@@ -1691,7 +1848,7 @@
       <c r="S47" s="3"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -1715,7 +1872,7 @@
       <c r="S48" s="9"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B49" s="16"/>
+      <c r="B49" s="17"/>
       <c r="C49" s="1" t="s">
         <v>4</v>
       </c>
@@ -1737,7 +1894,7 @@
       <c r="S49" s="3"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B50" s="15"/>
+      <c r="B50" s="18"/>
       <c r="C50" s="1" t="s">
         <v>5</v>
       </c>
@@ -1759,7 +1916,7 @@
       <c r="S50" s="3"/>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B51" s="15"/>
+      <c r="B51" s="18"/>
       <c r="C51" s="4" t="s">
         <v>6</v>
       </c>
@@ -1781,7 +1938,7 @@
       <c r="S51" s="3"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C52" s="7" t="s">
@@ -1805,7 +1962,7 @@
       <c r="S52" s="9"/>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B53" s="16"/>
+      <c r="B53" s="17"/>
       <c r="C53" s="1" t="s">
         <v>4</v>
       </c>
@@ -1827,7 +1984,7 @@
       <c r="S53" s="3"/>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B54" s="16"/>
+      <c r="B54" s="17"/>
       <c r="C54" s="1" t="s">
         <v>5</v>
       </c>
@@ -1849,7 +2006,7 @@
       <c r="S54" s="3"/>
     </row>
     <row r="55" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B55" s="20"/>
+      <c r="B55" s="19"/>
       <c r="C55" s="4" t="s">
         <v>6</v>
       </c>
@@ -1872,28 +2029,29 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="B48:B51"/>
     <mergeCell ref="B52:B55"/>
     <mergeCell ref="P34:S34"/>
     <mergeCell ref="B34:C35"/>
     <mergeCell ref="B36:B39"/>
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B47"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="B48:B51"/>
     <mergeCell ref="B28:B32"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="B6:C7"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="L34:O34"/>
-    <mergeCell ref="D34:G34"/>
     <mergeCell ref="B8:B12"/>
     <mergeCell ref="B23:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1901,7 +2059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -1909,18 +2067,18 @@
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="12"/>
     </row>
@@ -1928,38 +2086,38 @@
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="17" t="s">
+      <c r="B6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17" t="s">
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="10" t="s">
         <v>0</v>
       </c>
@@ -2010,8 +2168,8 @@
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="16" t="s">
-        <v>16</v>
+      <c r="B8" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
@@ -2034,7 +2192,7 @@
       <c r="S8" s="3"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="15"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
@@ -2056,7 +2214,7 @@
       <c r="S9" s="3"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="15"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -2078,7 +2236,7 @@
       <c r="S10" s="3"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="15"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
@@ -2100,7 +2258,7 @@
       <c r="S11" s="3"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="21"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
@@ -2122,7 +2280,7 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -2146,7 +2304,7 @@
       <c r="S13" s="9"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B14" s="15"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
@@ -2168,7 +2326,7 @@
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="15"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
@@ -2190,7 +2348,7 @@
       <c r="S15" s="3"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B16" s="15"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
@@ -2212,7 +2370,7 @@
       <c r="S16" s="3"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B17" s="21"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
@@ -2234,7 +2392,7 @@
       <c r="S17" s="6"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -2258,7 +2416,7 @@
       <c r="S18" s="9"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B19" s="15"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
@@ -2280,7 +2438,7 @@
       <c r="S19" s="3"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B20" s="15"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
@@ -2302,7 +2460,7 @@
       <c r="S20" s="3"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B21" s="15"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
@@ -2324,7 +2482,7 @@
       <c r="S21" s="3"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B22" s="21"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="4" t="s">
         <v>7</v>
       </c>
@@ -2346,7 +2504,7 @@
       <c r="S22" s="6"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -2370,7 +2528,7 @@
       <c r="S23" s="9"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B24" s="15"/>
+      <c r="B24" s="18"/>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
@@ -2392,7 +2550,7 @@
       <c r="S24" s="3"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B25" s="15"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
@@ -2414,7 +2572,7 @@
       <c r="S25" s="3"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B26" s="15"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
@@ -2436,7 +2594,7 @@
       <c r="S26" s="3"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B27" s="21"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="4" t="s">
         <v>7</v>
       </c>
@@ -2458,7 +2616,7 @@
       <c r="S27" s="6"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -2482,7 +2640,7 @@
       <c r="S28" s="9"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B29" s="16"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
@@ -2504,7 +2662,7 @@
       <c r="S29" s="3"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B30" s="16"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="1" t="s">
         <v>5</v>
       </c>
@@ -2526,7 +2684,7 @@
       <c r="S30" s="3"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B31" s="16"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="1" t="s">
         <v>6</v>
       </c>
@@ -2548,7 +2706,7 @@
       <c r="S31" s="3"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B32" s="20"/>
+      <c r="B32" s="19"/>
       <c r="C32" s="4" t="s">
         <v>7</v>
       </c>
@@ -2570,38 +2728,38 @@
       <c r="S32" s="6"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B34" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="17" t="s">
+      <c r="B34" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="20"/>
+      <c r="D34" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17" t="s">
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="17"/>
-      <c r="P34" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q34" s="17"/>
-      <c r="R34" s="17"/>
-      <c r="S34" s="17"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="15"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
       <c r="D35" s="10" t="s">
         <v>0</v>
       </c>
@@ -2652,8 +2810,8 @@
       </c>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B36" s="16" t="s">
-        <v>16</v>
+      <c r="B36" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>3</v>
@@ -2676,7 +2834,7 @@
       <c r="S36" s="3"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B37" s="16"/>
+      <c r="B37" s="17"/>
       <c r="C37" s="1" t="s">
         <v>4</v>
       </c>
@@ -2698,7 +2856,7 @@
       <c r="S37" s="3"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B38" s="15"/>
+      <c r="B38" s="18"/>
       <c r="C38" s="1" t="s">
         <v>5</v>
       </c>
@@ -2720,7 +2878,7 @@
       <c r="S38" s="3"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B39" s="15"/>
+      <c r="B39" s="18"/>
       <c r="C39" s="4" t="s">
         <v>6</v>
       </c>
@@ -2742,7 +2900,7 @@
       <c r="S39" s="3"/>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -2766,7 +2924,7 @@
       <c r="S40" s="9"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B41" s="16"/>
+      <c r="B41" s="17"/>
       <c r="C41" s="1" t="s">
         <v>4</v>
       </c>
@@ -2788,7 +2946,7 @@
       <c r="S41" s="3"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B42" s="15"/>
+      <c r="B42" s="18"/>
       <c r="C42" s="1" t="s">
         <v>5</v>
       </c>
@@ -2810,7 +2968,7 @@
       <c r="S42" s="3"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B43" s="15"/>
+      <c r="B43" s="18"/>
       <c r="C43" s="4" t="s">
         <v>6</v>
       </c>
@@ -2832,7 +2990,7 @@
       <c r="S43" s="3"/>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -2856,7 +3014,7 @@
       <c r="S44" s="9"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B45" s="16"/>
+      <c r="B45" s="17"/>
       <c r="C45" s="1" t="s">
         <v>4</v>
       </c>
@@ -2878,7 +3036,7 @@
       <c r="S45" s="3"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B46" s="15"/>
+      <c r="B46" s="18"/>
       <c r="C46" s="1" t="s">
         <v>5</v>
       </c>
@@ -2900,7 +3058,7 @@
       <c r="S46" s="3"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B47" s="15"/>
+      <c r="B47" s="18"/>
       <c r="C47" s="4" t="s">
         <v>6</v>
       </c>
@@ -2922,7 +3080,7 @@
       <c r="S47" s="3"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -2946,7 +3104,7 @@
       <c r="S48" s="9"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B49" s="16"/>
+      <c r="B49" s="17"/>
       <c r="C49" s="1" t="s">
         <v>4</v>
       </c>
@@ -2968,7 +3126,7 @@
       <c r="S49" s="3"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B50" s="15"/>
+      <c r="B50" s="18"/>
       <c r="C50" s="1" t="s">
         <v>5</v>
       </c>
@@ -2990,7 +3148,7 @@
       <c r="S50" s="3"/>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B51" s="15"/>
+      <c r="B51" s="18"/>
       <c r="C51" s="4" t="s">
         <v>6</v>
       </c>
@@ -3012,7 +3170,7 @@
       <c r="S51" s="3"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C52" s="7" t="s">
@@ -3036,7 +3194,7 @@
       <c r="S52" s="9"/>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B53" s="16"/>
+      <c r="B53" s="17"/>
       <c r="C53" s="1" t="s">
         <v>4</v>
       </c>
@@ -3058,7 +3216,7 @@
       <c r="S53" s="3"/>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B54" s="16"/>
+      <c r="B54" s="17"/>
       <c r="C54" s="1" t="s">
         <v>5</v>
       </c>
@@ -3080,7 +3238,7 @@
       <c r="S54" s="3"/>
     </row>
     <row r="55" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B55" s="20"/>
+      <c r="B55" s="19"/>
       <c r="C55" s="4" t="s">
         <v>6</v>
       </c>
@@ -3103,26 +3261,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="P34:S34"/>
     <mergeCell ref="B36:B39"/>
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B47"/>
     <mergeCell ref="B48:B51"/>
     <mergeCell ref="B52:B55"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="L34:O34"/>
-    <mergeCell ref="P34:S34"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="B6:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
distributedGrep running time updated
DistributedGrep running time updated
 * single node [1M1R]
 * Pseudo-DP [2M2R]
 * Pseudo-DP [4M2R]
 * Fully-DP [12M6R], partially

ageStdDev running time updated
 * single node [1M1R]
</commit_message>
<xml_diff>
--- a/doc/MR_RunningTime.xlsx
+++ b/doc/MR_RunningTime.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26124"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="980" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1.NumericalSummarization" sheetId="1" r:id="rId1"/>
@@ -59,6 +59,46 @@
           <t>stackoverflow.com users' data (1G)
 Pseudo-DP:
 ‘14 MacBook Pro, 2.8 GHz Intel Core i5    8GB 1600 MHz DDR3, 500GB SSD</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="D28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">#!/bin/bash
+beginTime=$(date '+%s')
+# command here
+hadoop jar jars/distributedGrep-0.0.1-SNAPSHOT.jar distributedGrep hdfs/Users.xml dg-out .*seoul.*
+endTime=$(date '+%s')
+elapsedTime=$(expr $endTime - $beginTime)
+echo TOTAL: $elapsedTime
+hadoop dfs -rmr dg-out
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
@@ -136,9 +176,6 @@
     <t>Fully-DP: RaspberryPi Cluster (3-node)</t>
   </si>
   <si>
-    <t>Distributed grep</t>
-  </si>
-  <si>
     <t>Bloom Filtering</t>
   </si>
   <si>
@@ -159,12 +196,15 @@
   <si>
     <t>Standard deviation of users' age</t>
   </si>
+  <si>
+    <t>Distributed grep with no Reduce function</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -212,6 +252,11 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
@@ -281,7 +326,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -306,28 +351,31 @@
     <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -611,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8:S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,38 +686,38 @@
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="21" t="s">
+      <c r="B6" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21" t="s">
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="14" t="s">
         <v>0</v>
       </c>
@@ -720,7 +768,7 @@
       </c>
     </row>
     <row r="8" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -743,16 +791,22 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="15"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
+      <c r="P8" s="2">
+        <v>173</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>173</v>
+      </c>
+      <c r="R8" s="2">
+        <v>174</v>
+      </c>
       <c r="S8" s="15">
         <f t="shared" ref="S8:S10" si="0">SUM(P8:R8)/3</f>
-        <v>0</v>
+        <v>173.33333333333334</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="24"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
@@ -773,16 +827,22 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="15"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
+      <c r="P9" s="2">
+        <v>88</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>89</v>
+      </c>
+      <c r="R9" s="2">
+        <v>88</v>
+      </c>
       <c r="S9" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>88.333333333333329</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="24"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -803,16 +863,22 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="15"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
+      <c r="P10" s="2">
+        <v>48</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>48</v>
+      </c>
+      <c r="R10" s="2">
+        <v>46</v>
+      </c>
       <c r="S10" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>47.333333333333336</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="24"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
@@ -833,16 +899,22 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="15"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
+      <c r="P11" s="2">
+        <v>27</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>27</v>
+      </c>
+      <c r="R11" s="2">
+        <v>26</v>
+      </c>
       <c r="S11" s="15">
         <f>SUM(P11:R11)/3</f>
-        <v>0</v>
+        <v>26.666666666666668</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="25"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
@@ -863,16 +935,22 @@
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="15"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
+      <c r="P12" s="5">
+        <v>24</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>23</v>
+      </c>
+      <c r="R12" s="5">
+        <v>26</v>
+      </c>
       <c r="S12" s="15">
         <f>SUM(P12:R12)/3</f>
-        <v>0</v>
+        <v>24.333333333333332</v>
       </c>
     </row>
     <row r="13" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -910,7 +988,7 @@
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B14" s="24"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
@@ -946,7 +1024,7 @@
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="24"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
@@ -982,7 +1060,7 @@
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B16" s="24"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
@@ -1018,7 +1096,7 @@
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B17" s="25"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
@@ -1054,7 +1132,7 @@
       </c>
     </row>
     <row r="18" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1090,7 +1168,7 @@
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B19" s="24"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1124,7 +1202,7 @@
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B20" s="24"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
@@ -1158,7 +1236,7 @@
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B21" s="24"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
@@ -1192,7 +1270,7 @@
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B22" s="25"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="4" t="s">
         <v>7</v>
       </c>
@@ -1226,7 +1304,7 @@
       </c>
     </row>
     <row r="23" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -1256,7 +1334,7 @@
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B24" s="24"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1286,7 +1364,7 @@
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B25" s="24"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
@@ -1316,7 +1394,7 @@
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B26" s="24"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
@@ -1346,7 +1424,7 @@
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B27" s="25"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="4" t="s">
         <v>7</v>
       </c>
@@ -1376,7 +1454,7 @@
       </c>
     </row>
     <row r="28" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -1406,7 +1484,7 @@
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B29" s="19"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
@@ -1436,7 +1514,7 @@
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B30" s="19"/>
+      <c r="B30" s="21"/>
       <c r="C30" s="1" t="s">
         <v>5</v>
       </c>
@@ -1466,7 +1544,7 @@
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B31" s="19"/>
+      <c r="B31" s="21"/>
       <c r="C31" s="1" t="s">
         <v>6</v>
       </c>
@@ -1496,7 +1574,7 @@
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B32" s="20"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="4" t="s">
         <v>7</v>
       </c>
@@ -1526,38 +1604,38 @@
       </c>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="25"/>
+      <c r="D34" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21" t="s">
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="M34" s="21"/>
-      <c r="N34" s="21"/>
-      <c r="O34" s="21"/>
-      <c r="P34" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q34" s="21"/>
-      <c r="R34" s="21"/>
-      <c r="S34" s="21"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
       <c r="D35" s="14" t="s">
         <v>0</v>
       </c>
@@ -1608,7 +1686,7 @@
       </c>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1632,7 +1710,7 @@
       <c r="S36" s="3"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B37" s="19"/>
+      <c r="B37" s="21"/>
       <c r="C37" s="1" t="s">
         <v>4</v>
       </c>
@@ -1654,7 +1732,7 @@
       <c r="S37" s="3"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B38" s="24"/>
+      <c r="B38" s="22"/>
       <c r="C38" s="1" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1754,7 @@
       <c r="S38" s="3"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B39" s="24"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="4" t="s">
         <v>6</v>
       </c>
@@ -1698,7 +1776,7 @@
       <c r="S39" s="3"/>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1722,7 +1800,7 @@
       <c r="S40" s="9"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B41" s="19"/>
+      <c r="B41" s="21"/>
       <c r="C41" s="1" t="s">
         <v>4</v>
       </c>
@@ -1744,7 +1822,7 @@
       <c r="S41" s="3"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B42" s="24"/>
+      <c r="B42" s="22"/>
       <c r="C42" s="1" t="s">
         <v>5</v>
       </c>
@@ -1766,7 +1844,7 @@
       <c r="S42" s="3"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B43" s="24"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="4" t="s">
         <v>6</v>
       </c>
@@ -1788,7 +1866,7 @@
       <c r="S43" s="3"/>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1812,7 +1890,7 @@
       <c r="S44" s="9"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B45" s="19"/>
+      <c r="B45" s="21"/>
       <c r="C45" s="1" t="s">
         <v>4</v>
       </c>
@@ -1834,7 +1912,7 @@
       <c r="S45" s="3"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B46" s="24"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="1" t="s">
         <v>5</v>
       </c>
@@ -1856,7 +1934,7 @@
       <c r="S46" s="3"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B47" s="24"/>
+      <c r="B47" s="22"/>
       <c r="C47" s="4" t="s">
         <v>6</v>
       </c>
@@ -1878,7 +1956,7 @@
       <c r="S47" s="3"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -1902,7 +1980,7 @@
       <c r="S48" s="9"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B49" s="19"/>
+      <c r="B49" s="21"/>
       <c r="C49" s="1" t="s">
         <v>4</v>
       </c>
@@ -1924,7 +2002,7 @@
       <c r="S49" s="3"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B50" s="24"/>
+      <c r="B50" s="22"/>
       <c r="C50" s="1" t="s">
         <v>5</v>
       </c>
@@ -1946,7 +2024,7 @@
       <c r="S50" s="3"/>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B51" s="24"/>
+      <c r="B51" s="22"/>
       <c r="C51" s="4" t="s">
         <v>6</v>
       </c>
@@ -1968,7 +2046,7 @@
       <c r="S51" s="3"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C52" s="7" t="s">
@@ -1992,7 +2070,7 @@
       <c r="S52" s="9"/>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B53" s="19"/>
+      <c r="B53" s="21"/>
       <c r="C53" s="1" t="s">
         <v>4</v>
       </c>
@@ -2014,7 +2092,7 @@
       <c r="S53" s="3"/>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B54" s="19"/>
+      <c r="B54" s="21"/>
       <c r="C54" s="1" t="s">
         <v>5</v>
       </c>
@@ -2036,7 +2114,7 @@
       <c r="S54" s="3"/>
     </row>
     <row r="55" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B55" s="20"/>
+      <c r="B55" s="23"/>
       <c r="C55" s="4" t="s">
         <v>6</v>
       </c>
@@ -2059,6 +2137,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="P34:S34"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="D34:G34"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="P6:S6"/>
@@ -2070,15 +2157,6 @@
     <mergeCell ref="B6:C7"/>
     <mergeCell ref="B8:B12"/>
     <mergeCell ref="B23:B27"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="P34:S34"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="L34:O34"/>
-    <mergeCell ref="D34:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2086,11 +2164,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2116,45 +2194,45 @@
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="21" t="s">
+      <c r="B6" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21" t="s">
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21" t="s">
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="10" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="18" t="s">
         <v>2</v>
       </c>
       <c r="G7" s="11" t="s">
@@ -2198,16 +2276,25 @@
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3"/>
+      <c r="D8" s="2">
+        <v>169</v>
+      </c>
+      <c r="E8" s="2">
+        <v>170</v>
+      </c>
+      <c r="F8" s="2">
+        <v>170</v>
+      </c>
+      <c r="G8" s="15">
+        <f t="shared" ref="G8:G10" si="0">SUM(D8:F8)/3</f>
+        <v>169.66666666666666</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -2222,14 +2309,23 @@
       <c r="S8" s="3"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="24"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3"/>
+      <c r="D9" s="2">
+        <v>86</v>
+      </c>
+      <c r="E9" s="2">
+        <v>86</v>
+      </c>
+      <c r="F9" s="2">
+        <v>85</v>
+      </c>
+      <c r="G9" s="15">
+        <f t="shared" si="0"/>
+        <v>85.666666666666671</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -2244,14 +2340,23 @@
       <c r="S9" s="3"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="24"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="3"/>
+      <c r="D10" s="2">
+        <v>43</v>
+      </c>
+      <c r="E10" s="2">
+        <v>43</v>
+      </c>
+      <c r="F10" s="2">
+        <v>43</v>
+      </c>
+      <c r="G10" s="15">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -2266,14 +2371,23 @@
       <c r="S10" s="3"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="24"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3"/>
+      <c r="D11" s="2">
+        <v>23</v>
+      </c>
+      <c r="E11" s="2">
+        <v>23</v>
+      </c>
+      <c r="F11" s="2">
+        <v>23</v>
+      </c>
+      <c r="G11" s="15">
+        <f>SUM(D11:F11)/3</f>
+        <v>23</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -2288,14 +2402,23 @@
       <c r="S11" s="3"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="25"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
+      <c r="D12" s="5">
+        <v>23</v>
+      </c>
+      <c r="E12" s="5">
+        <v>24</v>
+      </c>
+      <c r="F12" s="5">
+        <v>23</v>
+      </c>
+      <c r="G12" s="15">
+        <f>SUM(D12:F12)/3</f>
+        <v>23.333333333333332</v>
+      </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -2310,16 +2433,25 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9"/>
+      <c r="D13" s="8">
+        <v>169</v>
+      </c>
+      <c r="E13" s="8">
+        <v>162</v>
+      </c>
+      <c r="F13" s="8">
+        <v>187</v>
+      </c>
+      <c r="G13" s="15">
+        <f t="shared" ref="G13:G15" si="1">SUM(D13:F13)/3</f>
+        <v>172.66666666666666</v>
+      </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -2334,14 +2466,23 @@
       <c r="S13" s="9"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B14" s="24"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
+      <c r="D14" s="2">
+        <v>104</v>
+      </c>
+      <c r="E14" s="2">
+        <v>105</v>
+      </c>
+      <c r="F14" s="2">
+        <v>102</v>
+      </c>
+      <c r="G14" s="15">
+        <f t="shared" si="1"/>
+        <v>103.66666666666667</v>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -2356,14 +2497,23 @@
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="24"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="3"/>
+      <c r="D15" s="2">
+        <v>60</v>
+      </c>
+      <c r="E15" s="2">
+        <v>69</v>
+      </c>
+      <c r="F15" s="2">
+        <v>65</v>
+      </c>
+      <c r="G15" s="15">
+        <f t="shared" si="1"/>
+        <v>64.666666666666671</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -2378,14 +2528,23 @@
       <c r="S15" s="3"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B16" s="24"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="3"/>
+      <c r="D16" s="2">
+        <v>48</v>
+      </c>
+      <c r="E16" s="2">
+        <v>48</v>
+      </c>
+      <c r="F16" s="2">
+        <v>50</v>
+      </c>
+      <c r="G16" s="15">
+        <f>SUM(D16:F16)/3</f>
+        <v>48.666666666666664</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -2400,14 +2559,23 @@
       <c r="S16" s="3"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B17" s="25"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
+      <c r="D17" s="5">
+        <v>36</v>
+      </c>
+      <c r="E17" s="5">
+        <v>39</v>
+      </c>
+      <c r="F17" s="5">
+        <v>38</v>
+      </c>
+      <c r="G17" s="15">
+        <f>SUM(D17:F17)/3</f>
+        <v>37.666666666666664</v>
+      </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -2422,16 +2590,25 @@
       <c r="S17" s="6"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9"/>
+      <c r="D18" s="8">
+        <v>139</v>
+      </c>
+      <c r="E18" s="8">
+        <v>118</v>
+      </c>
+      <c r="F18" s="8">
+        <v>132</v>
+      </c>
+      <c r="G18" s="15">
+        <f t="shared" ref="G18:G20" si="2">SUM(D18:F18)/3</f>
+        <v>129.66666666666666</v>
+      </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -2446,14 +2623,23 @@
       <c r="S18" s="9"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B19" s="24"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="3"/>
+      <c r="D19" s="2">
+        <v>80</v>
+      </c>
+      <c r="E19" s="2">
+        <v>72</v>
+      </c>
+      <c r="F19" s="2">
+        <v>81</v>
+      </c>
+      <c r="G19" s="15">
+        <f t="shared" si="2"/>
+        <v>77.666666666666671</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -2468,14 +2654,23 @@
       <c r="S19" s="3"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B20" s="24"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="3"/>
+      <c r="D20" s="2">
+        <v>56</v>
+      </c>
+      <c r="E20" s="2">
+        <v>54</v>
+      </c>
+      <c r="F20" s="2">
+        <v>55</v>
+      </c>
+      <c r="G20" s="15">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -2490,14 +2685,23 @@
       <c r="S20" s="3"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B21" s="24"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="3"/>
+      <c r="D21" s="2">
+        <v>36</v>
+      </c>
+      <c r="E21" s="2">
+        <v>39</v>
+      </c>
+      <c r="F21" s="2">
+        <v>42</v>
+      </c>
+      <c r="G21" s="15">
+        <f>SUM(D21:F21)/3</f>
+        <v>39</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -2512,14 +2716,23 @@
       <c r="S21" s="3"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B22" s="25"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6"/>
+      <c r="D22" s="5">
+        <v>35</v>
+      </c>
+      <c r="E22" s="5">
+        <v>33</v>
+      </c>
+      <c r="F22" s="5">
+        <v>30</v>
+      </c>
+      <c r="G22" s="15">
+        <f>SUM(D22:F22)/3</f>
+        <v>32.666666666666664</v>
+      </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -2534,7 +2747,7 @@
       <c r="S22" s="6"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -2543,7 +2756,10 @@
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
-      <c r="G23" s="9"/>
+      <c r="G23" s="15">
+        <f t="shared" ref="G23:G25" si="3">SUM(D23:F23)/3</f>
+        <v>0</v>
+      </c>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -2558,14 +2774,17 @@
       <c r="S23" s="9"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B24" s="24"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2580,14 +2799,17 @@
       <c r="S24" s="3"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B25" s="24"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="3"/>
+      <c r="G25" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2602,14 +2824,17 @@
       <c r="S25" s="3"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B26" s="24"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="3"/>
+      <c r="G26" s="15">
+        <f>SUM(D26:F26)/3</f>
+        <v>0</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -2624,14 +2849,17 @@
       <c r="S26" s="3"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B27" s="25"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="6"/>
+      <c r="G27" s="15">
+        <f>SUM(D27:F27)/3</f>
+        <v>0</v>
+      </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
@@ -2646,7 +2874,7 @@
       <c r="S27" s="6"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -2655,7 +2883,10 @@
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="9"/>
+      <c r="G28" s="15">
+        <f t="shared" ref="G28:G30" si="4">SUM(D28:F28)/3</f>
+        <v>0</v>
+      </c>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
@@ -2670,14 +2901,19 @@
       <c r="S28" s="9"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B29" s="19"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2">
+        <v>250</v>
+      </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="3"/>
+      <c r="G29" s="15">
+        <f t="shared" si="4"/>
+        <v>83.333333333333329</v>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -2692,14 +2928,23 @@
       <c r="S29" s="3"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B30" s="19"/>
+      <c r="B30" s="21"/>
       <c r="C30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="3"/>
+      <c r="D30" s="2">
+        <v>335</v>
+      </c>
+      <c r="E30" s="2">
+        <v>359</v>
+      </c>
+      <c r="F30" s="2">
+        <v>341</v>
+      </c>
+      <c r="G30" s="15">
+        <f t="shared" si="4"/>
+        <v>345</v>
+      </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -2714,14 +2959,23 @@
       <c r="S30" s="3"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B31" s="19"/>
+      <c r="B31" s="21"/>
       <c r="C31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="3"/>
+      <c r="D31" s="2">
+        <v>336</v>
+      </c>
+      <c r="E31" s="2">
+        <v>357</v>
+      </c>
+      <c r="F31" s="2">
+        <v>326</v>
+      </c>
+      <c r="G31" s="15">
+        <f>SUM(D31:F31)/3</f>
+        <v>339.66666666666669</v>
+      </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -2736,14 +2990,23 @@
       <c r="S31" s="3"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B32" s="20"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="6"/>
+      <c r="D32" s="5">
+        <v>606</v>
+      </c>
+      <c r="E32" s="5">
+        <v>587</v>
+      </c>
+      <c r="F32" s="5">
+        <v>616</v>
+      </c>
+      <c r="G32" s="17">
+        <f>SUM(D32:F32)/3</f>
+        <v>603</v>
+      </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
@@ -2758,38 +3021,38 @@
       <c r="S32" s="6"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B34" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="21" t="s">
+      <c r="B34" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="25"/>
+      <c r="D34" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21" t="s">
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21" t="s">
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="M34" s="21"/>
-      <c r="N34" s="21"/>
-      <c r="O34" s="21"/>
-      <c r="P34" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q34" s="21"/>
-      <c r="R34" s="21"/>
-      <c r="S34" s="21"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
       <c r="D35" s="10" t="s">
         <v>0</v>
       </c>
@@ -2840,7 +3103,7 @@
       </c>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -2864,7 +3127,7 @@
       <c r="S36" s="3"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B37" s="19"/>
+      <c r="B37" s="21"/>
       <c r="C37" s="1" t="s">
         <v>4</v>
       </c>
@@ -2886,7 +3149,7 @@
       <c r="S37" s="3"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B38" s="24"/>
+      <c r="B38" s="22"/>
       <c r="C38" s="1" t="s">
         <v>5</v>
       </c>
@@ -2908,7 +3171,7 @@
       <c r="S38" s="3"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B39" s="24"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="4" t="s">
         <v>6</v>
       </c>
@@ -2930,7 +3193,7 @@
       <c r="S39" s="3"/>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -2954,7 +3217,7 @@
       <c r="S40" s="9"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B41" s="19"/>
+      <c r="B41" s="21"/>
       <c r="C41" s="1" t="s">
         <v>4</v>
       </c>
@@ -2976,7 +3239,7 @@
       <c r="S41" s="3"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B42" s="24"/>
+      <c r="B42" s="22"/>
       <c r="C42" s="1" t="s">
         <v>5</v>
       </c>
@@ -2998,7 +3261,7 @@
       <c r="S42" s="3"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B43" s="24"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="4" t="s">
         <v>6</v>
       </c>
@@ -3020,7 +3283,7 @@
       <c r="S43" s="3"/>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -3044,7 +3307,7 @@
       <c r="S44" s="9"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B45" s="19"/>
+      <c r="B45" s="21"/>
       <c r="C45" s="1" t="s">
         <v>4</v>
       </c>
@@ -3066,7 +3329,7 @@
       <c r="S45" s="3"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B46" s="24"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="1" t="s">
         <v>5</v>
       </c>
@@ -3088,7 +3351,7 @@
       <c r="S46" s="3"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B47" s="24"/>
+      <c r="B47" s="22"/>
       <c r="C47" s="4" t="s">
         <v>6</v>
       </c>
@@ -3110,7 +3373,7 @@
       <c r="S47" s="3"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -3134,7 +3397,7 @@
       <c r="S48" s="9"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B49" s="19"/>
+      <c r="B49" s="21"/>
       <c r="C49" s="1" t="s">
         <v>4</v>
       </c>
@@ -3156,7 +3419,7 @@
       <c r="S49" s="3"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B50" s="24"/>
+      <c r="B50" s="22"/>
       <c r="C50" s="1" t="s">
         <v>5</v>
       </c>
@@ -3178,7 +3441,7 @@
       <c r="S50" s="3"/>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B51" s="24"/>
+      <c r="B51" s="22"/>
       <c r="C51" s="4" t="s">
         <v>6</v>
       </c>
@@ -3200,7 +3463,7 @@
       <c r="S51" s="3"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C52" s="7" t="s">
@@ -3224,7 +3487,7 @@
       <c r="S52" s="9"/>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B53" s="19"/>
+      <c r="B53" s="21"/>
       <c r="C53" s="1" t="s">
         <v>4</v>
       </c>
@@ -3246,7 +3509,7 @@
       <c r="S53" s="3"/>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B54" s="19"/>
+      <c r="B54" s="21"/>
       <c r="C54" s="1" t="s">
         <v>5</v>
       </c>
@@ -3268,7 +3531,7 @@
       <c r="S54" s="3"/>
     </row>
     <row r="55" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B55" s="20"/>
+      <c r="B55" s="23"/>
       <c r="C55" s="4" t="s">
         <v>6</v>
       </c>
@@ -3291,28 +3554,29 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="P34:S34"/>
     <mergeCell ref="B36:B39"/>
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B47"/>
     <mergeCell ref="B48:B51"/>
     <mergeCell ref="B52:B55"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="L34:O34"/>
-    <mergeCell ref="P34:S34"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="B6:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Upload to result of test
using a variety of test case
</commit_message>
<xml_diff>
--- a/doc/MR_RunningTime.xlsx
+++ b/doc/MR_RunningTime.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="5600" yWindow="8820" windowWidth="14480" windowHeight="9180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="1.NumericalSummarization" sheetId="1" r:id="rId1"/>
@@ -47,28 +47,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="L8" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Redo </t>
-        </r>
-      </text>
-    </comment>
     <comment ref="P34" authorId="0">
       <text>
         <r>
@@ -96,29 +74,6 @@
           <t>stackoverflow.com users' data (1G)
 Pseudo-DP:
 ‘14 MacBook Pro, 2.8 GHz Intel Core i5    8GB 1600 MHz DDR3, 500GB SSD</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L36" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Redo
-</t>
         </r>
       </text>
     </comment>
@@ -355,7 +310,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,12 +368,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -527,12 +476,11 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -544,8 +492,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -568,21 +531,7 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -716,7 +665,7 @@
                   <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.33333333333331</c:v>
+                  <c:v>23.3333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -810,10 +759,10 @@
                   <c:v>64.66666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48.66666666666663</c:v>
+                  <c:v>48.66666666666661</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.66666666666663</c:v>
+                  <c:v>37.66666666666661</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -910,7 +859,7 @@
                   <c:v>39.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.66666666666663</c:v>
+                  <c:v>32.66666666666661</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -996,11 +945,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2078303568"/>
-        <c:axId val="2106963552"/>
+        <c:axId val="2105943056"/>
+        <c:axId val="2106911936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2078303568"/>
+        <c:axId val="2105943056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1043,7 +992,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2106963552"/>
+        <c:crossAx val="2106911936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1051,7 +1000,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106963552"/>
+        <c:axId val="2106911936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180.0"/>
@@ -1162,7 +1111,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2078303568"/>
+        <c:crossAx val="2105943056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="60.0"/>
@@ -1542,11 +1491,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2108574400"/>
-        <c:axId val="2108577744"/>
+        <c:axId val="2106984864"/>
+        <c:axId val="2106988224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2108574400"/>
+        <c:axId val="2106984864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1589,7 +1538,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108577744"/>
+        <c:crossAx val="2106988224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1597,7 +1546,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108577744"/>
+        <c:axId val="2106988224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600.0"/>
@@ -1708,7 +1657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108574400"/>
+        <c:crossAx val="2106984864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100.0"/>
@@ -3230,13 +3179,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AA60"/>
+  <dimension ref="A2:AD60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="11" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="16" max="23" width="10.83203125" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
@@ -3257,76 +3210,76 @@
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C5" s="12"/>
-      <c r="L5" s="50" t="s">
+      <c r="L5" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50" t="s">
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50" t="s">
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
-      <c r="W5" s="50"/>
-      <c r="X5" s="50" t="s">
+      <c r="U5" s="33"/>
+      <c r="V5" s="33"/>
+      <c r="W5" s="33"/>
+      <c r="X5" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="Y5" s="50"/>
-      <c r="Z5" s="50"/>
-      <c r="AA5" s="50"/>
+      <c r="Y5" s="33"/>
+      <c r="Z5" s="33"/>
+      <c r="AA5" s="33"/>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="35" t="s">
+      <c r="C6" s="40"/>
+      <c r="D6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35" t="s">
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35" t="s">
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35" t="s">
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
+      <c r="T6" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="U6" s="35"/>
-      <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-      <c r="X6" s="35" t="s">
+      <c r="U6" s="34"/>
+      <c r="V6" s="34"/>
+      <c r="W6" s="34"/>
+      <c r="X6" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="Y6" s="35"/>
-      <c r="Z6" s="35"/>
-      <c r="AA6" s="35"/>
+      <c r="Y6" s="34"/>
+      <c r="Z6" s="34"/>
+      <c r="AA6" s="34"/>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="14" t="s">
         <v>0</v>
       </c>
@@ -3401,7 +3354,7 @@
       </c>
     </row>
     <row r="8" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -3421,20 +3374,20 @@
         <v>172</v>
       </c>
       <c r="L8" s="20">
-        <f xml:space="preserve"> 13 * 60 +2</f>
-        <v>782</v>
+        <f>25 * 60 + 49</f>
+        <v>1549</v>
       </c>
       <c r="M8" s="20">
-        <f>13 * 60 + 4</f>
-        <v>784</v>
+        <f>25 * 60 + 49</f>
+        <v>1549</v>
       </c>
       <c r="N8" s="20">
-        <f xml:space="preserve"> 13 * 60 + 2</f>
-        <v>782</v>
+        <f xml:space="preserve"> 21* 60 + 49</f>
+        <v>1309</v>
       </c>
       <c r="O8" s="15">
         <f xml:space="preserve"> AVERAGE(L8,M8,N8)</f>
-        <v>782.66666666666663</v>
+        <v>1469</v>
       </c>
       <c r="P8" s="2">
         <v>173</v>
@@ -3465,16 +3418,25 @@
         <f xml:space="preserve"> AVERAGE(T8,U8,V8)</f>
         <v>1531</v>
       </c>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="21"/>
-      <c r="AA8" s="15" t="e">
+      <c r="X8" s="21">
+        <f>26 * 60 + 16</f>
+        <v>1576</v>
+      </c>
+      <c r="Y8" s="21">
+        <f>26 * 60 + 17</f>
+        <v>1577</v>
+      </c>
+      <c r="Z8" s="21">
+        <f>26 * 60 + 20</f>
+        <v>1580</v>
+      </c>
+      <c r="AA8" s="15">
         <f xml:space="preserve"> AVERAGE(X8,Y8,Z8)</f>
-        <v>#DIV/0!</v>
+        <v>1577.6666666666667</v>
       </c>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B9" s="46"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
@@ -3536,16 +3498,25 @@
         <f t="shared" ref="W9:W22" si="3" xml:space="preserve"> AVERAGE(T9,U9,V9)</f>
         <v>767</v>
       </c>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
-      <c r="AA9" s="15" t="e">
+      <c r="X9" s="21">
+        <f>13*60 +26</f>
+        <v>806</v>
+      </c>
+      <c r="Y9" s="21">
+        <f>13 * 60 + 27</f>
+        <v>807</v>
+      </c>
+      <c r="Z9" s="21">
+        <f>13 * 60 + 30</f>
+        <v>810</v>
+      </c>
+      <c r="AA9" s="15">
         <f t="shared" ref="AA9:AA22" si="4" xml:space="preserve"> AVERAGE(X9,Y9,Z9)</f>
-        <v>#DIV/0!</v>
+        <v>807.66666666666663</v>
       </c>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B10" s="46"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -3607,16 +3578,25 @@
         <f t="shared" si="3"/>
         <v>386.33333333333331</v>
       </c>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="15" t="e">
+      <c r="X10" s="21">
+        <f>7 * 60 + 11</f>
+        <v>431</v>
+      </c>
+      <c r="Y10" s="21">
+        <f>7 * 60 + 2</f>
+        <v>422</v>
+      </c>
+      <c r="Z10" s="21">
+        <f>7 * 60 + 2</f>
+        <v>422</v>
+      </c>
+      <c r="AA10" s="15">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>425</v>
       </c>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B11" s="46"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
@@ -3678,16 +3658,25 @@
         <f t="shared" si="3"/>
         <v>265.33333333333331</v>
       </c>
-      <c r="X11" s="21"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="21"/>
-      <c r="AA11" s="15" t="e">
+      <c r="X11" s="21">
+        <f>6 * 60 + 50</f>
+        <v>410</v>
+      </c>
+      <c r="Y11" s="21">
+        <f>6 * 60 + 47</f>
+        <v>407</v>
+      </c>
+      <c r="Z11" s="21">
+        <f>6 * 60 + 56</f>
+        <v>416</v>
+      </c>
+      <c r="AA11" s="15">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>411</v>
       </c>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B12" s="47"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
@@ -3749,16 +3738,25 @@
         <f t="shared" si="3"/>
         <v>211</v>
       </c>
-      <c r="X12" s="22"/>
-      <c r="Y12" s="22"/>
-      <c r="Z12" s="22"/>
-      <c r="AA12" s="15" t="e">
+      <c r="X12" s="22">
+        <f>5*60 + 17</f>
+        <v>317</v>
+      </c>
+      <c r="Y12" s="22">
+        <f>5 * 60 +  14</f>
+        <v>314</v>
+      </c>
+      <c r="Z12" s="22">
+        <f>5 * 60 + 6</f>
+        <v>306</v>
+      </c>
+      <c r="AA12" s="15">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>312.33333333333331</v>
       </c>
     </row>
     <row r="13" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -3822,16 +3820,25 @@
         <f t="shared" si="3"/>
         <v>1553.3333333333333</v>
       </c>
-      <c r="X13" s="23"/>
-      <c r="Y13" s="23"/>
-      <c r="Z13" s="23"/>
-      <c r="AA13" s="15" t="e">
+      <c r="X13" s="23">
+        <f>26 * 60 + 29</f>
+        <v>1589</v>
+      </c>
+      <c r="Y13" s="23">
+        <f>26 * 60 + 30</f>
+        <v>1590</v>
+      </c>
+      <c r="Z13" s="23">
+        <f>26 * 60 + 20</f>
+        <v>1580</v>
+      </c>
+      <c r="AA13" s="15">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1586.3333333333333</v>
       </c>
     </row>
     <row r="14" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B14" s="46"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
@@ -3893,16 +3900,25 @@
         <f t="shared" si="3"/>
         <v>793</v>
       </c>
-      <c r="X14" s="21"/>
-      <c r="Y14" s="21"/>
-      <c r="Z14" s="21"/>
-      <c r="AA14" s="15" t="e">
+      <c r="X14" s="21">
+        <f>13 * 60 + 45</f>
+        <v>825</v>
+      </c>
+      <c r="Y14" s="21">
+        <f>13 * 60 + 45</f>
+        <v>825</v>
+      </c>
+      <c r="Z14" s="21">
+        <f>14 * 60 + 3</f>
+        <v>843</v>
+      </c>
+      <c r="AA14" s="15">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>831</v>
       </c>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B15" s="46"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
@@ -3964,16 +3980,25 @@
         <f t="shared" si="3"/>
         <v>596.33333333333337</v>
       </c>
-      <c r="X15" s="21"/>
-      <c r="Y15" s="21"/>
-      <c r="Z15" s="21"/>
-      <c r="AA15" s="15" t="e">
+      <c r="X15" s="21">
+        <f>10 * 60 + 31</f>
+        <v>631</v>
+      </c>
+      <c r="Y15" s="21">
+        <f>10 * 60 + 29</f>
+        <v>629</v>
+      </c>
+      <c r="Z15" s="21">
+        <f>10 * 60 + 42</f>
+        <v>642</v>
+      </c>
+      <c r="AA15" s="15">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>634</v>
       </c>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="46"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
@@ -4035,16 +4060,25 @@
         <f t="shared" si="3"/>
         <v>349</v>
       </c>
-      <c r="X16" s="21"/>
-      <c r="Y16" s="21"/>
-      <c r="Z16" s="21"/>
-      <c r="AA16" s="15" t="e">
+      <c r="X16" s="21">
+        <f xml:space="preserve"> 8 * 60 + 3</f>
+        <v>483</v>
+      </c>
+      <c r="Y16" s="21">
+        <f>7 * 60 + 23</f>
+        <v>443</v>
+      </c>
+      <c r="Z16" s="21">
+        <f>7 * 60 + 17</f>
+        <v>437</v>
+      </c>
+      <c r="AA16" s="15">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>454.33333333333331</v>
       </c>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B17" s="47"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
@@ -4106,16 +4140,25 @@
         <f t="shared" si="3"/>
         <v>266</v>
       </c>
-      <c r="X17" s="22"/>
-      <c r="Y17" s="22"/>
-      <c r="Z17" s="22"/>
-      <c r="AA17" s="15" t="e">
+      <c r="X17" s="22">
+        <f>4 * 60 + 54</f>
+        <v>294</v>
+      </c>
+      <c r="Y17" s="22">
+        <f>5 * 60 + 6</f>
+        <v>306</v>
+      </c>
+      <c r="Z17" s="22">
+        <f>4 * 60 + 57</f>
+        <v>297</v>
+      </c>
+      <c r="AA17" s="15">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>299</v>
       </c>
     </row>
     <row r="18" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -4177,16 +4220,25 @@
         <f t="shared" si="3"/>
         <v>1571.6666666666667</v>
       </c>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="23"/>
-      <c r="Z18" s="23"/>
-      <c r="AA18" s="15" t="e">
+      <c r="X18" s="23">
+        <f>26 * 60 +42</f>
+        <v>1602</v>
+      </c>
+      <c r="Y18" s="23">
+        <f>26 * 60 + 26</f>
+        <v>1586</v>
+      </c>
+      <c r="Z18" s="23">
+        <f>26 * 60 + 22</f>
+        <v>1582</v>
+      </c>
+      <c r="AA18" s="15">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B19" s="46"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
@@ -4246,16 +4298,25 @@
         <f t="shared" si="3"/>
         <v>598</v>
       </c>
-      <c r="X19" s="21"/>
-      <c r="Y19" s="21"/>
-      <c r="Z19" s="21"/>
-      <c r="AA19" s="15" t="e">
+      <c r="X19" s="21">
+        <f xml:space="preserve"> 13* 60 + 33</f>
+        <v>813</v>
+      </c>
+      <c r="Y19" s="21">
+        <f>13 * 60 + 19</f>
+        <v>799</v>
+      </c>
+      <c r="Z19" s="21">
+        <f>13 * 60 + 19</f>
+        <v>799</v>
+      </c>
+      <c r="AA19" s="15">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>803.66666666666663</v>
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B20" s="46"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
@@ -4315,16 +4376,25 @@
         <f t="shared" si="3"/>
         <v>595.66666666666663</v>
       </c>
-      <c r="X20" s="21"/>
-      <c r="Y20" s="21"/>
-      <c r="Z20" s="21"/>
-      <c r="AA20" s="15" t="e">
+      <c r="X20" s="21">
+        <f xml:space="preserve"> 8 * 60 + 15</f>
+        <v>495</v>
+      </c>
+      <c r="Y20" s="21">
+        <f>9 * 60 +10</f>
+        <v>550</v>
+      </c>
+      <c r="Z20" s="21">
+        <f xml:space="preserve"> 9 * 60 + 36</f>
+        <v>576</v>
+      </c>
+      <c r="AA20" s="15">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>540.33333333333337</v>
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B21" s="46"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
@@ -4384,16 +4454,25 @@
         <f t="shared" si="3"/>
         <v>348</v>
       </c>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
-      <c r="Z21" s="21"/>
-      <c r="AA21" s="15" t="e">
+      <c r="X21" s="21">
+        <f>6 * 60 + 30</f>
+        <v>390</v>
+      </c>
+      <c r="Y21" s="21">
+        <f>6 * 60 + 16</f>
+        <v>376</v>
+      </c>
+      <c r="Z21" s="21">
+        <f>7 * 60 + 7</f>
+        <v>427</v>
+      </c>
+      <c r="AA21" s="15">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>397.66666666666669</v>
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B22" s="47"/>
+      <c r="B22" s="39"/>
       <c r="C22" s="4" t="s">
         <v>7</v>
       </c>
@@ -4453,16 +4532,25 @@
         <f t="shared" si="3"/>
         <v>263</v>
       </c>
-      <c r="X22" s="22"/>
-      <c r="Y22" s="22"/>
-      <c r="Z22" s="22"/>
-      <c r="AA22" s="15" t="e">
+      <c r="X22" s="22">
+        <f>5 * 60 + 46</f>
+        <v>346</v>
+      </c>
+      <c r="Y22" s="22">
+        <f>5*60+14</f>
+        <v>314</v>
+      </c>
+      <c r="Z22" s="22">
+        <f>5*60+9</f>
+        <v>309</v>
+      </c>
+      <c r="AA22" s="15">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="35" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -4506,7 +4594,7 @@
       <c r="AA23" s="15"/>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B24" s="46"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
@@ -4550,7 +4638,7 @@
       <c r="AA24" s="15"/>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B25" s="46"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
@@ -4594,7 +4682,7 @@
       <c r="AA25" s="15"/>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B26" s="46"/>
+      <c r="B26" s="37"/>
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
@@ -4638,7 +4726,7 @@
       <c r="AA26" s="15"/>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B27" s="47"/>
+      <c r="B27" s="39"/>
       <c r="C27" s="4" t="s">
         <v>7</v>
       </c>
@@ -4682,7 +4770,7 @@
       <c r="AA27" s="15"/>
     </row>
     <row r="28" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -4726,7 +4814,7 @@
       <c r="AA28" s="15"/>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B29" s="37"/>
+      <c r="B29" s="36"/>
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
@@ -4764,7 +4852,7 @@
       <c r="AA29" s="15"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B30" s="37"/>
+      <c r="B30" s="36"/>
       <c r="C30" s="1" t="s">
         <v>5</v>
       </c>
@@ -4802,7 +4890,7 @@
       <c r="AA30" s="15"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B31" s="37"/>
+      <c r="B31" s="36"/>
       <c r="C31" s="1" t="s">
         <v>6</v>
       </c>
@@ -4877,73 +4965,73 @@
       <c r="Z32" s="5"/>
       <c r="AA32" s="17"/>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="L33" s="50" t="s">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="L33" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="M33" s="50"/>
-      <c r="N33" s="50"/>
-      <c r="O33" s="50"/>
-      <c r="T33" s="50" t="s">
+      <c r="M33" s="33"/>
+      <c r="N33" s="33"/>
+      <c r="O33" s="33"/>
+      <c r="T33" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="U33" s="50"/>
-      <c r="V33" s="50"/>
-      <c r="W33" s="50"/>
-      <c r="X33" s="50" t="s">
+      <c r="U33" s="33"/>
+      <c r="V33" s="33"/>
+      <c r="W33" s="33"/>
+      <c r="X33" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="Y33" s="50"/>
-      <c r="Z33" s="50"/>
-      <c r="AA33" s="50"/>
-    </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Y33" s="33"/>
+      <c r="Z33" s="33"/>
+      <c r="AA33" s="33"/>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="12"/>
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="34" t="s">
+      <c r="C34" s="43"/>
+      <c r="D34" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34" t="s">
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="34" t="s">
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="M34" s="34"/>
-      <c r="N34" s="34"/>
-      <c r="O34" s="34"/>
-      <c r="P34" s="35" t="s">
+      <c r="M34" s="42"/>
+      <c r="N34" s="42"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="Q34" s="35"/>
-      <c r="R34" s="35"/>
-      <c r="S34" s="35"/>
-      <c r="T34" s="34" t="s">
+      <c r="Q34" s="34"/>
+      <c r="R34" s="34"/>
+      <c r="S34" s="34"/>
+      <c r="T34" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="U34" s="34"/>
-      <c r="V34" s="34"/>
-      <c r="W34" s="34"/>
-      <c r="X34" s="34" t="s">
+      <c r="U34" s="42"/>
+      <c r="V34" s="42"/>
+      <c r="W34" s="42"/>
+      <c r="X34" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="Y34" s="34"/>
-      <c r="Z34" s="34"/>
-      <c r="AA34" s="34"/>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Y34" s="42"/>
+      <c r="Z34" s="42"/>
+      <c r="AA34" s="42"/>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="12"/>
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
       <c r="D35" s="24" t="s">
         <v>0</v>
       </c>
@@ -5017,9 +5105,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="12"/>
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="45" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="26">
@@ -5033,22 +5121,25 @@
       <c r="I36" s="27"/>
       <c r="J36" s="27"/>
       <c r="K36" s="28"/>
-      <c r="L36" s="29">
-        <v>806</v>
-      </c>
-      <c r="M36" s="29">
-        <v>807</v>
-      </c>
-      <c r="N36" s="29">
-        <v>807</v>
-      </c>
-      <c r="O36" s="30">
+      <c r="L36" s="27">
+        <f>13 * 60 + 22</f>
+        <v>802</v>
+      </c>
+      <c r="M36" s="27">
+        <f>13 * 60 + 24</f>
+        <v>804</v>
+      </c>
+      <c r="N36" s="27">
+        <f>13 * 60 + 24</f>
+        <v>804</v>
+      </c>
+      <c r="O36" s="29">
         <v>806.67</v>
       </c>
       <c r="P36" s="27"/>
       <c r="Q36" s="27"/>
       <c r="R36" s="27"/>
-      <c r="S36" s="30"/>
+      <c r="S36" s="29"/>
       <c r="T36" s="27">
         <v>768</v>
       </c>
@@ -5058,19 +5149,28 @@
       <c r="V36" s="27">
         <v>768</v>
       </c>
-      <c r="W36" s="30">
+      <c r="W36" s="29">
         <v>767.67</v>
       </c>
-      <c r="X36" s="27"/>
-      <c r="Y36" s="27"/>
-      <c r="Z36" s="27"/>
-      <c r="AA36" s="30" t="e">
+      <c r="X36" s="27">
+        <f>14 * 60 + 33</f>
+        <v>873</v>
+      </c>
+      <c r="Y36" s="27">
+        <f>14*60 + 30</f>
+        <v>870</v>
+      </c>
+      <c r="Z36" s="27">
+        <f>14 * 60 +33</f>
+        <v>873</v>
+      </c>
+      <c r="AA36" s="29" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="12"/>
-      <c r="B37" s="42"/>
+      <c r="B37" s="46"/>
       <c r="C37" s="26">
         <v>40</v>
       </c>
@@ -5091,13 +5191,13 @@
       <c r="N37" s="27">
         <v>792</v>
       </c>
-      <c r="O37" s="30">
+      <c r="O37" s="29">
         <v>792.33</v>
       </c>
       <c r="P37" s="27"/>
       <c r="Q37" s="27"/>
       <c r="R37" s="27"/>
-      <c r="S37" s="30"/>
+      <c r="S37" s="29"/>
       <c r="T37" s="27">
         <v>768</v>
       </c>
@@ -5107,19 +5207,28 @@
       <c r="V37" s="27">
         <v>768</v>
       </c>
-      <c r="W37" s="30">
+      <c r="W37" s="29">
         <v>768</v>
       </c>
-      <c r="X37" s="27"/>
-      <c r="Y37" s="27"/>
-      <c r="Z37" s="27"/>
-      <c r="AA37" s="30" t="e">
+      <c r="X37" s="27">
+        <f>13 * 60 + 45</f>
+        <v>825</v>
+      </c>
+      <c r="Y37" s="27">
+        <f>13 * 60 + 48</f>
+        <v>828</v>
+      </c>
+      <c r="Z37" s="27">
+        <f>13 * 60 + 48</f>
+        <v>828</v>
+      </c>
+      <c r="AA37" s="29" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:30" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="12"/>
-      <c r="B38" s="42"/>
+      <c r="B38" s="46"/>
       <c r="C38" s="26">
         <v>80</v>
       </c>
@@ -5140,13 +5249,13 @@
       <c r="N38" s="27">
         <v>783</v>
       </c>
-      <c r="O38" s="30">
+      <c r="O38" s="29">
         <v>784.67</v>
       </c>
       <c r="P38" s="27"/>
       <c r="Q38" s="27"/>
       <c r="R38" s="27"/>
-      <c r="S38" s="30"/>
+      <c r="S38" s="29"/>
       <c r="T38" s="27">
         <v>767</v>
       </c>
@@ -5156,19 +5265,28 @@
       <c r="V38" s="27">
         <v>768</v>
       </c>
-      <c r="W38" s="30">
+      <c r="W38" s="29">
         <v>767.33</v>
       </c>
-      <c r="X38" s="27"/>
-      <c r="Y38" s="27"/>
-      <c r="Z38" s="27"/>
-      <c r="AA38" s="30" t="e">
+      <c r="X38" s="27">
+        <f>13 * 60 + 36</f>
+        <v>816</v>
+      </c>
+      <c r="Y38" s="27">
+        <f>13 * 60 + 33</f>
+        <v>813</v>
+      </c>
+      <c r="Z38" s="27">
+        <f>13 * 60 + 33</f>
+        <v>813</v>
+      </c>
+      <c r="AA38" s="29" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" s="12"/>
-      <c r="B39" s="42"/>
+      <c r="B39" s="46"/>
       <c r="C39" s="26">
         <v>160</v>
       </c>
@@ -5189,13 +5307,13 @@
       <c r="N39" s="27">
         <v>786</v>
       </c>
-      <c r="O39" s="30">
+      <c r="O39" s="29">
         <v>782.67</v>
       </c>
       <c r="P39" s="27"/>
       <c r="Q39" s="27"/>
       <c r="R39" s="27"/>
-      <c r="S39" s="30"/>
+      <c r="S39" s="29"/>
       <c r="T39" s="27">
         <v>768</v>
       </c>
@@ -5205,20 +5323,29 @@
       <c r="V39" s="27">
         <v>768</v>
       </c>
-      <c r="W39" s="30">
+      <c r="W39" s="29">
         <v>768</v>
       </c>
-      <c r="X39" s="27"/>
-      <c r="Y39" s="27"/>
-      <c r="Z39" s="27"/>
-      <c r="AA39" s="30" t="e">
+      <c r="X39" s="27">
+        <f>13 * 60 + 18</f>
+        <v>798</v>
+      </c>
+      <c r="Y39" s="27">
+        <f>13 * 60 + 18</f>
+        <v>798</v>
+      </c>
+      <c r="Z39" s="27">
+        <f>13 * 60 + 18</f>
+        <v>798</v>
+      </c>
+      <c r="AA39" s="29" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="12"/>
-      <c r="B40" s="43"/>
-      <c r="C40" s="31">
+      <c r="B40" s="47"/>
+      <c r="C40" s="30">
         <v>320</v>
       </c>
       <c r="D40" s="27"/>
@@ -5238,13 +5365,13 @@
       <c r="N40" s="27">
         <v>780</v>
       </c>
-      <c r="O40" s="30">
+      <c r="O40" s="29">
         <v>780</v>
       </c>
       <c r="P40" s="27"/>
       <c r="Q40" s="27"/>
       <c r="R40" s="27"/>
-      <c r="S40" s="30"/>
+      <c r="S40" s="29"/>
       <c r="T40" s="27">
         <v>768</v>
       </c>
@@ -5254,76 +5381,88 @@
       <c r="V40" s="27">
         <v>767</v>
       </c>
-      <c r="W40" s="30">
+      <c r="W40" s="29">
         <v>767.67</v>
       </c>
-      <c r="X40" s="27"/>
-      <c r="Y40" s="27"/>
-      <c r="Z40" s="27"/>
-      <c r="AA40" s="30" t="e">
+      <c r="X40" s="27">
+        <f>13 * 60 + 18</f>
+        <v>798</v>
+      </c>
+      <c r="Y40" s="27">
+        <f>13 * 60 + 29</f>
+        <v>809</v>
+      </c>
+      <c r="Z40" s="27">
+        <f>13 * 60 + 24</f>
+        <v>804</v>
+      </c>
+      <c r="AA40" s="29" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="12"/>
-      <c r="B41" s="44" t="s">
+      <c r="B41" s="48" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="26">
         <v>20</v>
       </c>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="33"/>
-      <c r="L41" s="32">
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="32"/>
+      <c r="L41" s="31">
         <v>637</v>
       </c>
-      <c r="M41" s="32">
+      <c r="M41" s="31">
         <v>609</v>
       </c>
-      <c r="N41" s="32">
+      <c r="N41" s="31">
         <v>610</v>
       </c>
-      <c r="O41" s="30">
+      <c r="O41" s="29">
         <v>618.66999999999996</v>
       </c>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="32"/>
-      <c r="R41" s="32"/>
-      <c r="S41" s="30"/>
-      <c r="T41" s="32">
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="S41" s="29"/>
+      <c r="T41" s="31">
         <v>597</v>
       </c>
-      <c r="U41" s="32">
+      <c r="U41" s="31">
         <v>597</v>
       </c>
-      <c r="V41" s="32">
+      <c r="V41" s="31">
         <v>594</v>
       </c>
-      <c r="W41" s="30">
+      <c r="W41" s="29">
         <v>596</v>
       </c>
-      <c r="X41" s="32">
+      <c r="X41" s="31">
         <v>629</v>
       </c>
-      <c r="Y41" s="32">
+      <c r="Y41" s="31">
         <v>666</v>
       </c>
-      <c r="Z41" s="32">
+      <c r="Z41" s="31">
         <v>688</v>
       </c>
-      <c r="AA41" s="30">
+      <c r="AA41" s="29">
         <v>661</v>
       </c>
-    </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB41" s="50"/>
+      <c r="AC41" s="50"/>
+      <c r="AD41" s="50"/>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="12"/>
-      <c r="B42" s="45"/>
+      <c r="B42" s="49"/>
       <c r="C42" s="26">
         <v>40</v>
       </c>
@@ -5344,13 +5483,13 @@
       <c r="N42" s="27">
         <v>607</v>
       </c>
-      <c r="O42" s="30">
+      <c r="O42" s="29">
         <v>609.33000000000004</v>
       </c>
       <c r="P42" s="27"/>
       <c r="Q42" s="27"/>
       <c r="R42" s="27"/>
-      <c r="S42" s="30"/>
+      <c r="S42" s="29"/>
       <c r="T42" s="27">
         <v>597</v>
       </c>
@@ -5360,7 +5499,7 @@
       <c r="V42" s="27">
         <v>596</v>
       </c>
-      <c r="W42" s="30">
+      <c r="W42" s="29">
         <v>599.33000000000004</v>
       </c>
       <c r="X42" s="27">
@@ -5372,13 +5511,13 @@
       <c r="Z42" s="27">
         <v>640</v>
       </c>
-      <c r="AA42" s="30">
+      <c r="AA42" s="29">
         <v>638.66999999999996</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="12"/>
-      <c r="B43" s="45"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="26">
         <v>80</v>
       </c>
@@ -5399,13 +5538,13 @@
       <c r="N43" s="27">
         <v>641</v>
       </c>
-      <c r="O43" s="30">
+      <c r="O43" s="29">
         <v>618.33000000000004</v>
       </c>
       <c r="P43" s="27"/>
       <c r="Q43" s="27"/>
       <c r="R43" s="27"/>
-      <c r="S43" s="30"/>
+      <c r="S43" s="29"/>
       <c r="T43" s="27">
         <v>596</v>
       </c>
@@ -5415,21 +5554,30 @@
       <c r="V43" s="27">
         <v>611</v>
       </c>
-      <c r="W43" s="30">
+      <c r="W43" s="29">
         <v>600.66999999999996</v>
       </c>
-      <c r="X43" s="27"/>
-      <c r="Y43" s="27"/>
-      <c r="Z43" s="27"/>
-      <c r="AA43" s="30" t="e">
+      <c r="X43" s="27">
+        <f>10 * 60 + 33</f>
+        <v>633</v>
+      </c>
+      <c r="Y43" s="27">
+        <f>10 * 60 + 29</f>
+        <v>629</v>
+      </c>
+      <c r="Z43" s="27">
+        <f>10 * 60 + 34</f>
+        <v>634</v>
+      </c>
+      <c r="AA43" s="29" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="45"/>
+      <c r="B44" s="49"/>
       <c r="C44" s="26">
         <v>160</v>
       </c>
@@ -5450,13 +5598,13 @@
       <c r="N44" s="27">
         <v>613</v>
       </c>
-      <c r="O44" s="30">
+      <c r="O44" s="29">
         <v>613.66999999999996</v>
       </c>
       <c r="P44" s="27"/>
       <c r="Q44" s="27"/>
       <c r="R44" s="27"/>
-      <c r="S44" s="30"/>
+      <c r="S44" s="29"/>
       <c r="T44" s="27">
         <v>604</v>
       </c>
@@ -5466,20 +5614,29 @@
       <c r="V44" s="27">
         <v>597</v>
       </c>
-      <c r="W44" s="30">
+      <c r="W44" s="29">
         <v>599.33000000000004</v>
       </c>
-      <c r="X44" s="27"/>
-      <c r="Y44" s="27"/>
-      <c r="Z44" s="27"/>
-      <c r="AA44" s="30" t="e">
+      <c r="X44" s="27">
+        <f>10*60 +30</f>
+        <v>630</v>
+      </c>
+      <c r="Y44" s="27">
+        <f>10 * 60 + 30</f>
+        <v>630</v>
+      </c>
+      <c r="Z44" s="27">
+        <f>10 * 60 + 29</f>
+        <v>629</v>
+      </c>
+      <c r="AA44" s="29" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" s="12"/>
-      <c r="B45" s="43"/>
-      <c r="C45" s="31">
+      <c r="B45" s="47"/>
+      <c r="C45" s="30">
         <v>320</v>
       </c>
       <c r="D45" s="27"/>
@@ -5499,13 +5656,13 @@
       <c r="N45" s="27">
         <v>547</v>
       </c>
-      <c r="O45" s="30">
+      <c r="O45" s="29">
         <v>540</v>
       </c>
       <c r="P45" s="27"/>
       <c r="Q45" s="27"/>
       <c r="R45" s="27"/>
-      <c r="S45" s="30"/>
+      <c r="S45" s="29"/>
       <c r="T45" s="27">
         <v>597</v>
       </c>
@@ -5515,70 +5672,88 @@
       <c r="V45" s="27">
         <v>596</v>
       </c>
-      <c r="W45" s="30">
+      <c r="W45" s="29">
         <v>596.66999999999996</v>
       </c>
-      <c r="X45" s="27"/>
-      <c r="Y45" s="27"/>
-      <c r="Z45" s="27"/>
-      <c r="AA45" s="30" t="e">
+      <c r="X45" s="27">
+        <f>10 * 60 + 29</f>
+        <v>629</v>
+      </c>
+      <c r="Y45" s="27">
+        <f xml:space="preserve"> 10 * 60 + 29</f>
+        <v>629</v>
+      </c>
+      <c r="Z45" s="27">
+        <f>10 * 60 + 31</f>
+        <v>631</v>
+      </c>
+      <c r="AA45" s="29" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="12"/>
-      <c r="B46" s="44" t="s">
+      <c r="B46" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C46" s="26">
         <v>20</v>
       </c>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
-      <c r="K46" s="33"/>
-      <c r="L46" s="32">
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="31"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
+      <c r="K46" s="32"/>
+      <c r="L46" s="31">
         <v>615</v>
       </c>
-      <c r="M46" s="32">
+      <c r="M46" s="31">
         <v>612</v>
       </c>
-      <c r="N46" s="32">
+      <c r="N46" s="31">
         <v>614</v>
       </c>
-      <c r="O46" s="30">
+      <c r="O46" s="29">
         <v>613.66999999999996</v>
       </c>
-      <c r="P46" s="32"/>
-      <c r="Q46" s="32"/>
-      <c r="R46" s="32"/>
-      <c r="S46" s="30"/>
-      <c r="T46" s="32">
+      <c r="P46" s="31"/>
+      <c r="Q46" s="31"/>
+      <c r="R46" s="31"/>
+      <c r="S46" s="29"/>
+      <c r="T46" s="31">
         <v>596</v>
       </c>
-      <c r="U46" s="32">
+      <c r="U46" s="31">
         <v>595</v>
       </c>
-      <c r="V46" s="32">
+      <c r="V46" s="31">
         <v>596</v>
       </c>
-      <c r="W46" s="30">
+      <c r="W46" s="29">
         <v>595.66999999999996</v>
       </c>
-      <c r="X46" s="32"/>
-      <c r="Y46" s="32"/>
-      <c r="Z46" s="32"/>
-      <c r="AA46" s="30" t="e">
+      <c r="X46" s="31">
+        <f>10 * 60 + 36</f>
+        <v>636</v>
+      </c>
+      <c r="Y46" s="31">
+        <f>10*60+32</f>
+        <v>632</v>
+      </c>
+      <c r="Z46" s="31">
+        <f>10 * 60 +33</f>
+        <v>633</v>
+      </c>
+      <c r="AA46" s="29" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="12"/>
-      <c r="B47" s="45"/>
+      <c r="B47" s="49"/>
       <c r="C47" s="26">
         <v>40</v>
       </c>
@@ -5599,13 +5774,13 @@
       <c r="N47" s="27">
         <v>612</v>
       </c>
-      <c r="O47" s="30">
+      <c r="O47" s="29">
         <v>612.33000000000004</v>
       </c>
       <c r="P47" s="27"/>
       <c r="Q47" s="27"/>
       <c r="R47" s="27"/>
-      <c r="S47" s="30"/>
+      <c r="S47" s="29"/>
       <c r="T47" s="27">
         <v>595</v>
       </c>
@@ -5615,19 +5790,28 @@
       <c r="V47" s="27">
         <v>595</v>
       </c>
-      <c r="W47" s="30">
+      <c r="W47" s="29">
         <v>595</v>
       </c>
-      <c r="X47" s="27"/>
-      <c r="Y47" s="27"/>
-      <c r="Z47" s="27"/>
-      <c r="AA47" s="30" t="e">
+      <c r="X47" s="27">
+        <f>10 * 60 + 44</f>
+        <v>644</v>
+      </c>
+      <c r="Y47" s="27">
+        <f>10 * 60 + 42</f>
+        <v>642</v>
+      </c>
+      <c r="Z47" s="27">
+        <f>10 * 60 + 37</f>
+        <v>637</v>
+      </c>
+      <c r="AA47" s="29" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="12"/>
-      <c r="B48" s="45"/>
+      <c r="B48" s="49"/>
       <c r="C48" s="26">
         <v>80</v>
       </c>
@@ -5648,13 +5832,13 @@
       <c r="N48" s="27">
         <v>613</v>
       </c>
-      <c r="O48" s="30">
+      <c r="O48" s="29">
         <v>613.66999999999996</v>
       </c>
       <c r="P48" s="27"/>
       <c r="Q48" s="27"/>
       <c r="R48" s="27"/>
-      <c r="S48" s="30"/>
+      <c r="S48" s="29"/>
       <c r="T48" s="27">
         <v>596</v>
       </c>
@@ -5664,19 +5848,28 @@
       <c r="V48" s="27">
         <v>595</v>
       </c>
-      <c r="W48" s="30">
+      <c r="W48" s="29">
         <v>595.33000000000004</v>
       </c>
-      <c r="X48" s="27"/>
-      <c r="Y48" s="27"/>
-      <c r="Z48" s="27"/>
-      <c r="AA48" s="30" t="e">
+      <c r="X48" s="27">
+        <f>10 * 60 + 32</f>
+        <v>632</v>
+      </c>
+      <c r="Y48" s="27">
+        <f>10 * 60 + 31</f>
+        <v>631</v>
+      </c>
+      <c r="Z48" s="27">
+        <f>10 * 60 + 44</f>
+        <v>644</v>
+      </c>
+      <c r="AA48" s="29" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A49" s="12"/>
-      <c r="B49" s="45"/>
+      <c r="B49" s="49"/>
       <c r="C49" s="26">
         <v>160</v>
       </c>
@@ -5697,13 +5890,13 @@
       <c r="N49" s="27">
         <v>614</v>
       </c>
-      <c r="O49" s="30">
+      <c r="O49" s="29">
         <v>613</v>
       </c>
       <c r="P49" s="27"/>
       <c r="Q49" s="27"/>
       <c r="R49" s="27"/>
-      <c r="S49" s="30"/>
+      <c r="S49" s="29"/>
       <c r="T49" s="27">
         <v>601</v>
       </c>
@@ -5713,20 +5906,29 @@
       <c r="V49" s="27">
         <v>597</v>
       </c>
-      <c r="W49" s="30">
+      <c r="W49" s="29">
         <v>598</v>
       </c>
-      <c r="X49" s="27"/>
-      <c r="Y49" s="27"/>
-      <c r="Z49" s="27"/>
-      <c r="AA49" s="30" t="e">
+      <c r="X49" s="27">
+        <f>10 * 60 + 29</f>
+        <v>629</v>
+      </c>
+      <c r="Y49" s="27">
+        <f>10 * 60 + 29</f>
+        <v>629</v>
+      </c>
+      <c r="Z49" s="27">
+        <f>10 * 60 + 30</f>
+        <v>630</v>
+      </c>
+      <c r="AA49" s="29" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A50" s="12"/>
-      <c r="B50" s="43"/>
-      <c r="C50" s="31">
+      <c r="B50" s="47"/>
+      <c r="C50" s="30">
         <v>320</v>
       </c>
       <c r="D50" s="27"/>
@@ -5765,15 +5967,24 @@
       <c r="W50" s="28">
         <v>599.33000000000004</v>
       </c>
-      <c r="X50" s="27"/>
-      <c r="Y50" s="27"/>
-      <c r="Z50" s="27"/>
+      <c r="X50" s="27">
+        <f xml:space="preserve"> 10*60+29</f>
+        <v>629</v>
+      </c>
+      <c r="Y50" s="27">
+        <f>10 * 60 + 29</f>
+        <v>629</v>
+      </c>
+      <c r="Z50" s="27">
+        <f>10 * 60 + 29</f>
+        <v>629</v>
+      </c>
       <c r="AA50" s="28" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B51" s="36" t="s">
+      <c r="B51" s="35" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="26">
@@ -5805,7 +6016,7 @@
       <c r="AA51" s="9"/>
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B52" s="37"/>
+      <c r="B52" s="36"/>
       <c r="C52" s="26">
         <v>40</v>
       </c>
@@ -5835,7 +6046,7 @@
       <c r="AA52" s="3"/>
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B53" s="37"/>
+      <c r="B53" s="36"/>
       <c r="C53" s="26">
         <v>80</v>
       </c>
@@ -5865,7 +6076,7 @@
       <c r="AA53" s="3"/>
     </row>
     <row r="54" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B54" s="46"/>
+      <c r="B54" s="37"/>
       <c r="C54" s="26">
         <v>160</v>
       </c>
@@ -5895,8 +6106,8 @@
       <c r="AA54" s="3"/>
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B55" s="46"/>
-      <c r="C55" s="31">
+      <c r="B55" s="37"/>
+      <c r="C55" s="30">
         <v>320</v>
       </c>
       <c r="D55" s="2"/>
@@ -5925,7 +6136,7 @@
       <c r="AA55" s="3"/>
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B56" s="36" t="s">
+      <c r="B56" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C56" s="26">
@@ -5957,7 +6168,7 @@
       <c r="AA56" s="9"/>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B57" s="37"/>
+      <c r="B57" s="36"/>
       <c r="C57" s="26">
         <v>40</v>
       </c>
@@ -5987,7 +6198,7 @@
       <c r="AA57" s="3"/>
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B58" s="37"/>
+      <c r="B58" s="36"/>
       <c r="C58" s="26">
         <v>80</v>
       </c>
@@ -6017,7 +6228,7 @@
       <c r="AA58" s="3"/>
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B59" s="37"/>
+      <c r="B59" s="36"/>
       <c r="C59" s="26">
         <v>160</v>
       </c>
@@ -6048,7 +6259,7 @@
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B60" s="38"/>
-      <c r="C60" s="31">
+      <c r="C60" s="30">
         <v>320</v>
       </c>
       <c r="D60" s="5"/>
@@ -6078,21 +6289,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="T33:W33"/>
-    <mergeCell ref="L33:O33"/>
-    <mergeCell ref="X33:AA33"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B23:B27"/>
     <mergeCell ref="T34:W34"/>
     <mergeCell ref="X34:AA34"/>
     <mergeCell ref="T6:W6"/>
@@ -6109,6 +6305,21 @@
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="P6:S6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="T33:W33"/>
+    <mergeCell ref="L33:O33"/>
+    <mergeCell ref="X33:AA33"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="P5:S5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6146,38 +6357,38 @@
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="35" t="s">
+      <c r="C6" s="40"/>
+      <c r="D6" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35" t="s">
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35" t="s">
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="18" t="s">
         <v>0</v>
       </c>
@@ -6228,7 +6439,7 @@
       </c>
     </row>
     <row r="8" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -6261,7 +6472,7 @@
       <c r="S8" s="3"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="46"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
@@ -6292,7 +6503,7 @@
       <c r="S9" s="3"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="46"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -6323,7 +6534,7 @@
       <c r="S10" s="3"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="46"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
@@ -6354,7 +6565,7 @@
       <c r="S11" s="3"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="47"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
@@ -6385,7 +6596,7 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -6418,7 +6629,7 @@
       <c r="S13" s="9"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B14" s="46"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
@@ -6449,7 +6660,7 @@
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="46"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
@@ -6480,7 +6691,7 @@
       <c r="S15" s="3"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B16" s="46"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
@@ -6511,7 +6722,7 @@
       <c r="S16" s="3"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B17" s="47"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
@@ -6542,7 +6753,7 @@
       <c r="S17" s="6"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -6575,7 +6786,7 @@
       <c r="S18" s="9"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B19" s="46"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
@@ -6606,7 +6817,7 @@
       <c r="S19" s="3"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B20" s="46"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
@@ -6637,7 +6848,7 @@
       <c r="S20" s="3"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B21" s="46"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
@@ -6668,7 +6879,7 @@
       <c r="S21" s="3"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B22" s="47"/>
+      <c r="B22" s="39"/>
       <c r="C22" s="4" t="s">
         <v>7</v>
       </c>
@@ -6699,7 +6910,7 @@
       <c r="S22" s="6"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="35" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -6732,7 +6943,7 @@
       <c r="S23" s="9"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B24" s="46"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
@@ -6763,7 +6974,7 @@
       <c r="S24" s="3"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B25" s="46"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
@@ -6794,7 +7005,7 @@
       <c r="S25" s="3"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B26" s="46"/>
+      <c r="B26" s="37"/>
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
@@ -6825,7 +7036,7 @@
       <c r="S26" s="3"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B27" s="47"/>
+      <c r="B27" s="39"/>
       <c r="C27" s="4" t="s">
         <v>7</v>
       </c>
@@ -6856,7 +7067,7 @@
       <c r="S27" s="6"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -6889,7 +7100,7 @@
       <c r="S28" s="9"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B29" s="37"/>
+      <c r="B29" s="36"/>
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
@@ -6920,7 +7131,7 @@
       <c r="S29" s="3"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B30" s="37"/>
+      <c r="B30" s="36"/>
       <c r="C30" s="1" t="s">
         <v>5</v>
       </c>
@@ -6951,7 +7162,7 @@
       <c r="S30" s="3"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B31" s="37"/>
+      <c r="B31" s="36"/>
       <c r="C31" s="1" t="s">
         <v>6</v>
       </c>
@@ -7013,38 +7224,38 @@
       <c r="S32" s="6"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B34" s="48" t="s">
+      <c r="B34" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="48"/>
-      <c r="D34" s="35" t="s">
+      <c r="C34" s="40"/>
+      <c r="D34" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35" t="s">
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="I34" s="35"/>
-      <c r="J34" s="35"/>
-      <c r="K34" s="35"/>
-      <c r="L34" s="35" t="s">
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="M34" s="35"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="35"/>
-      <c r="P34" s="35" t="s">
+      <c r="M34" s="34"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="34"/>
+      <c r="P34" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="Q34" s="35"/>
-      <c r="R34" s="35"/>
-      <c r="S34" s="35"/>
+      <c r="Q34" s="34"/>
+      <c r="R34" s="34"/>
+      <c r="S34" s="34"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
       <c r="D35" s="10" t="s">
         <v>0</v>
       </c>
@@ -7095,7 +7306,7 @@
       </c>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -7119,7 +7330,7 @@
       <c r="S36" s="3"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B37" s="37"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="1" t="s">
         <v>4</v>
       </c>
@@ -7141,7 +7352,7 @@
       <c r="S37" s="3"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B38" s="46"/>
+      <c r="B38" s="37"/>
       <c r="C38" s="1" t="s">
         <v>5</v>
       </c>
@@ -7163,7 +7374,7 @@
       <c r="S38" s="3"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B39" s="46"/>
+      <c r="B39" s="37"/>
       <c r="C39" s="4" t="s">
         <v>6</v>
       </c>
@@ -7185,7 +7396,7 @@
       <c r="S39" s="3"/>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -7209,7 +7420,7 @@
       <c r="S40" s="9"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B41" s="37"/>
+      <c r="B41" s="36"/>
       <c r="C41" s="1" t="s">
         <v>4</v>
       </c>
@@ -7231,7 +7442,7 @@
       <c r="S41" s="3"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B42" s="46"/>
+      <c r="B42" s="37"/>
       <c r="C42" s="1" t="s">
         <v>5</v>
       </c>
@@ -7253,7 +7464,7 @@
       <c r="S42" s="3"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B43" s="46"/>
+      <c r="B43" s="37"/>
       <c r="C43" s="4" t="s">
         <v>6</v>
       </c>
@@ -7275,7 +7486,7 @@
       <c r="S43" s="3"/>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B44" s="36" t="s">
+      <c r="B44" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -7299,7 +7510,7 @@
       <c r="S44" s="9"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B45" s="37"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="1" t="s">
         <v>4</v>
       </c>
@@ -7321,7 +7532,7 @@
       <c r="S45" s="3"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B46" s="46"/>
+      <c r="B46" s="37"/>
       <c r="C46" s="1" t="s">
         <v>5</v>
       </c>
@@ -7343,7 +7554,7 @@
       <c r="S46" s="3"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B47" s="46"/>
+      <c r="B47" s="37"/>
       <c r="C47" s="4" t="s">
         <v>6</v>
       </c>
@@ -7365,7 +7576,7 @@
       <c r="S47" s="3"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B48" s="36" t="s">
+      <c r="B48" s="35" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -7389,7 +7600,7 @@
       <c r="S48" s="9"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B49" s="37"/>
+      <c r="B49" s="36"/>
       <c r="C49" s="1" t="s">
         <v>4</v>
       </c>
@@ -7411,7 +7622,7 @@
       <c r="S49" s="3"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B50" s="46"/>
+      <c r="B50" s="37"/>
       <c r="C50" s="1" t="s">
         <v>5</v>
       </c>
@@ -7433,7 +7644,7 @@
       <c r="S50" s="3"/>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B51" s="46"/>
+      <c r="B51" s="37"/>
       <c r="C51" s="4" t="s">
         <v>6</v>
       </c>
@@ -7455,7 +7666,7 @@
       <c r="S51" s="3"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B52" s="36" t="s">
+      <c r="B52" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C52" s="7" t="s">
@@ -7479,7 +7690,7 @@
       <c r="S52" s="9"/>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B53" s="37"/>
+      <c r="B53" s="36"/>
       <c r="C53" s="1" t="s">
         <v>4</v>
       </c>
@@ -7501,7 +7712,7 @@
       <c r="S53" s="3"/>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B54" s="37"/>
+      <c r="B54" s="36"/>
       <c r="C54" s="1" t="s">
         <v>5</v>
       </c>
@@ -7546,26 +7757,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="P34:S34"/>
     <mergeCell ref="B36:B39"/>
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B47"/>
     <mergeCell ref="B48:B51"/>
     <mergeCell ref="B52:B55"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="L34:O34"/>
-    <mergeCell ref="P34:S34"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="B6:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Upload to revised documents
MR_RunningTime.xlsx is revised
</commit_message>
<xml_diff>
--- a/doc/MR_RunningTime.xlsx
+++ b/doc/MR_RunningTime.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="8820" windowWidth="14480" windowHeight="9180" tabRatio="500"/>
+    <workbookView xWindow="840" yWindow="460" windowWidth="27960" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="1.NumericalSummarization" sheetId="1" r:id="rId1"/>
@@ -480,7 +480,8 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -492,23 +493,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -531,7 +517,21 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -665,7 +665,7 @@
                   <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.3333333333333</c:v>
+                  <c:v>23.33333333333329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -759,10 +759,10 @@
                   <c:v>64.66666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48.66666666666661</c:v>
+                  <c:v>48.66666666666659</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.66666666666661</c:v>
+                  <c:v>37.66666666666659</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -859,7 +859,7 @@
                   <c:v>39.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.66666666666661</c:v>
+                  <c:v>32.66666666666659</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -945,11 +945,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2105943056"/>
-        <c:axId val="2106911936"/>
+        <c:axId val="-2128930544"/>
+        <c:axId val="2138113680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2105943056"/>
+        <c:axId val="-2128930544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -992,7 +992,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2106911936"/>
+        <c:crossAx val="2138113680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1000,7 +1000,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106911936"/>
+        <c:axId val="2138113680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180.0"/>
@@ -1111,7 +1111,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2105943056"/>
+        <c:crossAx val="-2128930544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="60.0"/>
@@ -1491,11 +1491,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2106984864"/>
-        <c:axId val="2106988224"/>
+        <c:axId val="-2127045488"/>
+        <c:axId val="-2128850432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2106984864"/>
+        <c:axId val="-2127045488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1538,7 +1538,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2106988224"/>
+        <c:crossAx val="-2128850432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1546,7 +1546,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106988224"/>
+        <c:axId val="-2128850432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600.0"/>
@@ -1657,7 +1657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2106984864"/>
+        <c:crossAx val="-2127045488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100.0"/>
@@ -3181,14 +3181,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AD60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="11" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="16" max="23" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="4" max="19" width="10.83203125" customWidth="1"/>
+    <col min="20" max="23" width="10.83203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:27" x14ac:dyDescent="0.2">
@@ -3210,76 +3210,76 @@
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C5" s="12"/>
-      <c r="L5" s="33" t="s">
+      <c r="L5" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33" t="s">
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33" t="s">
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="50"/>
+      <c r="T5" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="U5" s="33"/>
-      <c r="V5" s="33"/>
-      <c r="W5" s="33"/>
-      <c r="X5" s="33" t="s">
+      <c r="U5" s="50"/>
+      <c r="V5" s="50"/>
+      <c r="W5" s="50"/>
+      <c r="X5" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="Y5" s="33"/>
-      <c r="Z5" s="33"/>
-      <c r="AA5" s="33"/>
+      <c r="Y5" s="50"/>
+      <c r="Z5" s="50"/>
+      <c r="AA5" s="50"/>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="34" t="s">
+      <c r="C6" s="48"/>
+      <c r="D6" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34" t="s">
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34" t="s">
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="34"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34" t="s">
+      <c r="Q6" s="35"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="U6" s="34"/>
-      <c r="V6" s="34"/>
-      <c r="W6" s="34"/>
-      <c r="X6" s="34" t="s">
+      <c r="U6" s="35"/>
+      <c r="V6" s="35"/>
+      <c r="W6" s="35"/>
+      <c r="X6" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="Y6" s="34"/>
-      <c r="Z6" s="34"/>
-      <c r="AA6" s="34"/>
+      <c r="Y6" s="35"/>
+      <c r="Z6" s="35"/>
+      <c r="AA6" s="35"/>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="14" t="s">
         <v>0</v>
       </c>
@@ -3354,7 +3354,7 @@
       </c>
     </row>
     <row r="8" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="37" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -3436,7 +3436,7 @@
       </c>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B9" s="37"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
@@ -3516,7 +3516,7 @@
       </c>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B10" s="37"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -3596,7 +3596,7 @@
       </c>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B11" s="37"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
@@ -3676,7 +3676,7 @@
       </c>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B12" s="39"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
@@ -3756,7 +3756,7 @@
       </c>
     </row>
     <row r="13" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="36" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -3838,7 +3838,7 @@
       </c>
     </row>
     <row r="14" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B14" s="37"/>
+      <c r="B14" s="46"/>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
@@ -3918,7 +3918,7 @@
       </c>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B15" s="37"/>
+      <c r="B15" s="46"/>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
@@ -3998,7 +3998,7 @@
       </c>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="37"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
@@ -4078,7 +4078,7 @@
       </c>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B17" s="39"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
@@ -4158,7 +4158,7 @@
       </c>
     </row>
     <row r="18" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="36" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -4238,7 +4238,7 @@
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B19" s="37"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
@@ -4316,7 +4316,7 @@
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B20" s="37"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
@@ -4394,7 +4394,7 @@
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B21" s="37"/>
+      <c r="B21" s="46"/>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
@@ -4472,7 +4472,7 @@
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B22" s="39"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="4" t="s">
         <v>7</v>
       </c>
@@ -4550,7 +4550,7 @@
       </c>
     </row>
     <row r="23" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -4594,7 +4594,7 @@
       <c r="AA23" s="15"/>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B24" s="37"/>
+      <c r="B24" s="46"/>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
@@ -4638,7 +4638,7 @@
       <c r="AA24" s="15"/>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B25" s="37"/>
+      <c r="B25" s="46"/>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
@@ -4682,7 +4682,7 @@
       <c r="AA25" s="15"/>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B26" s="37"/>
+      <c r="B26" s="46"/>
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
@@ -4726,7 +4726,7 @@
       <c r="AA26" s="15"/>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B27" s="39"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="4" t="s">
         <v>7</v>
       </c>
@@ -4770,7 +4770,7 @@
       <c r="AA27" s="15"/>
     </row>
     <row r="28" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -4814,7 +4814,7 @@
       <c r="AA28" s="15"/>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B29" s="36"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
@@ -4852,7 +4852,7 @@
       <c r="AA29" s="15"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B30" s="36"/>
+      <c r="B30" s="37"/>
       <c r="C30" s="1" t="s">
         <v>5</v>
       </c>
@@ -4890,7 +4890,7 @@
       <c r="AA30" s="15"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B31" s="36"/>
+      <c r="B31" s="37"/>
       <c r="C31" s="1" t="s">
         <v>6</v>
       </c>
@@ -4966,72 +4966,72 @@
       <c r="AA32" s="17"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="L33" s="33" t="s">
+      <c r="L33" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
-      <c r="O33" s="33"/>
-      <c r="T33" s="33" t="s">
+      <c r="M33" s="50"/>
+      <c r="N33" s="50"/>
+      <c r="O33" s="50"/>
+      <c r="T33" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="U33" s="33"/>
-      <c r="V33" s="33"/>
-      <c r="W33" s="33"/>
-      <c r="X33" s="33" t="s">
+      <c r="U33" s="50"/>
+      <c r="V33" s="50"/>
+      <c r="W33" s="50"/>
+      <c r="X33" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="Y33" s="33"/>
-      <c r="Z33" s="33"/>
-      <c r="AA33" s="33"/>
+      <c r="Y33" s="50"/>
+      <c r="Z33" s="50"/>
+      <c r="AA33" s="50"/>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="12"/>
-      <c r="B34" s="43" t="s">
+      <c r="B34" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="43"/>
-      <c r="D34" s="42" t="s">
+      <c r="C34" s="39"/>
+      <c r="D34" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42" t="s">
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="I34" s="42"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="42"/>
-      <c r="L34" s="42" t="s">
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="M34" s="42"/>
-      <c r="N34" s="42"/>
-      <c r="O34" s="42"/>
-      <c r="P34" s="34" t="s">
+      <c r="M34" s="34"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="34"/>
+      <c r="P34" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="Q34" s="34"/>
-      <c r="R34" s="34"/>
-      <c r="S34" s="34"/>
-      <c r="T34" s="42" t="s">
+      <c r="Q34" s="35"/>
+      <c r="R34" s="35"/>
+      <c r="S34" s="35"/>
+      <c r="T34" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="U34" s="42"/>
-      <c r="V34" s="42"/>
-      <c r="W34" s="42"/>
-      <c r="X34" s="42" t="s">
+      <c r="U34" s="34"/>
+      <c r="V34" s="34"/>
+      <c r="W34" s="34"/>
+      <c r="X34" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="Y34" s="42"/>
-      <c r="Z34" s="42"/>
-      <c r="AA34" s="42"/>
+      <c r="Y34" s="34"/>
+      <c r="Z34" s="34"/>
+      <c r="AA34" s="34"/>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="12"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
       <c r="D35" s="24" t="s">
         <v>0</v>
       </c>
@@ -5107,7 +5107,7 @@
     </row>
     <row r="36" spans="1:30" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="12"/>
-      <c r="B36" s="45" t="s">
+      <c r="B36" s="41" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="26">
@@ -5164,13 +5164,14 @@
         <f>14 * 60 +33</f>
         <v>873</v>
       </c>
-      <c r="AA36" s="29" t="e">
-        <v>#DIV/0!</v>
+      <c r="AA36" s="15">
+        <f xml:space="preserve"> AVERAGE(X36,Y36,Z36)</f>
+        <v>872</v>
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="12"/>
-      <c r="B37" s="46"/>
+      <c r="B37" s="42"/>
       <c r="C37" s="26">
         <v>40</v>
       </c>
@@ -5222,13 +5223,14 @@
         <f>13 * 60 + 48</f>
         <v>828</v>
       </c>
-      <c r="AA37" s="29" t="e">
-        <v>#DIV/0!</v>
+      <c r="AA37" s="15">
+        <f t="shared" ref="AA37:AA50" si="9" xml:space="preserve"> AVERAGE(X37,Y37,Z37)</f>
+        <v>827</v>
       </c>
     </row>
     <row r="38" spans="1:30" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="12"/>
-      <c r="B38" s="46"/>
+      <c r="B38" s="42"/>
       <c r="C38" s="26">
         <v>80</v>
       </c>
@@ -5280,13 +5282,14 @@
         <f>13 * 60 + 33</f>
         <v>813</v>
       </c>
-      <c r="AA38" s="29" t="e">
-        <v>#DIV/0!</v>
+      <c r="AA38" s="15">
+        <f t="shared" si="9"/>
+        <v>814</v>
       </c>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" s="12"/>
-      <c r="B39" s="46"/>
+      <c r="B39" s="42"/>
       <c r="C39" s="26">
         <v>160</v>
       </c>
@@ -5338,13 +5341,14 @@
         <f>13 * 60 + 18</f>
         <v>798</v>
       </c>
-      <c r="AA39" s="29" t="e">
-        <v>#DIV/0!</v>
+      <c r="AA39" s="15">
+        <f t="shared" si="9"/>
+        <v>798</v>
       </c>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="12"/>
-      <c r="B40" s="47"/>
+      <c r="B40" s="43"/>
       <c r="C40" s="30">
         <v>320</v>
       </c>
@@ -5396,13 +5400,14 @@
         <f>13 * 60 + 24</f>
         <v>804</v>
       </c>
-      <c r="AA40" s="29" t="e">
-        <v>#DIV/0!</v>
+      <c r="AA40" s="15">
+        <f t="shared" si="9"/>
+        <v>803.66666666666663</v>
       </c>
     </row>
     <row r="41" spans="1:30" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="12"/>
-      <c r="B41" s="48" t="s">
+      <c r="B41" s="44" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="26">
@@ -5453,16 +5458,17 @@
       <c r="Z41" s="31">
         <v>688</v>
       </c>
-      <c r="AA41" s="29">
+      <c r="AA41" s="15">
+        <f t="shared" si="9"/>
         <v>661</v>
       </c>
-      <c r="AB41" s="50"/>
-      <c r="AC41" s="50"/>
-      <c r="AD41" s="50"/>
+      <c r="AB41" s="33"/>
+      <c r="AC41" s="33"/>
+      <c r="AD41" s="33"/>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="12"/>
-      <c r="B42" s="49"/>
+      <c r="B42" s="45"/>
       <c r="C42" s="26">
         <v>40</v>
       </c>
@@ -5511,13 +5517,14 @@
       <c r="Z42" s="27">
         <v>640</v>
       </c>
-      <c r="AA42" s="29">
-        <v>638.66999999999996</v>
+      <c r="AA42" s="15">
+        <f t="shared" si="9"/>
+        <v>638.66666666666663</v>
       </c>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="12"/>
-      <c r="B43" s="49"/>
+      <c r="B43" s="45"/>
       <c r="C43" s="26">
         <v>80</v>
       </c>
@@ -5569,15 +5576,16 @@
         <f>10 * 60 + 34</f>
         <v>634</v>
       </c>
-      <c r="AA43" s="29" t="e">
-        <v>#DIV/0!</v>
+      <c r="AA43" s="15">
+        <f t="shared" si="9"/>
+        <v>632</v>
       </c>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="49"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="26">
         <v>160</v>
       </c>
@@ -5629,13 +5637,14 @@
         <f>10 * 60 + 29</f>
         <v>629</v>
       </c>
-      <c r="AA44" s="29" t="e">
-        <v>#DIV/0!</v>
+      <c r="AA44" s="15">
+        <f t="shared" si="9"/>
+        <v>629.66666666666663</v>
       </c>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" s="12"/>
-      <c r="B45" s="47"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="30">
         <v>320</v>
       </c>
@@ -5687,13 +5696,14 @@
         <f>10 * 60 + 31</f>
         <v>631</v>
       </c>
-      <c r="AA45" s="29" t="e">
-        <v>#DIV/0!</v>
+      <c r="AA45" s="15">
+        <f t="shared" si="9"/>
+        <v>629.66666666666663</v>
       </c>
     </row>
     <row r="46" spans="1:30" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="12"/>
-      <c r="B46" s="48" t="s">
+      <c r="B46" s="44" t="s">
         <v>10</v>
       </c>
       <c r="C46" s="26">
@@ -5747,13 +5757,14 @@
         <f>10 * 60 +33</f>
         <v>633</v>
       </c>
-      <c r="AA46" s="29" t="e">
-        <v>#DIV/0!</v>
+      <c r="AA46" s="15">
+        <f t="shared" si="9"/>
+        <v>633.66666666666663</v>
       </c>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="12"/>
-      <c r="B47" s="49"/>
+      <c r="B47" s="45"/>
       <c r="C47" s="26">
         <v>40</v>
       </c>
@@ -5805,13 +5816,14 @@
         <f>10 * 60 + 37</f>
         <v>637</v>
       </c>
-      <c r="AA47" s="29" t="e">
-        <v>#DIV/0!</v>
+      <c r="AA47" s="15">
+        <f t="shared" si="9"/>
+        <v>641</v>
       </c>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="12"/>
-      <c r="B48" s="49"/>
+      <c r="B48" s="45"/>
       <c r="C48" s="26">
         <v>80</v>
       </c>
@@ -5863,13 +5875,14 @@
         <f>10 * 60 + 44</f>
         <v>644</v>
       </c>
-      <c r="AA48" s="29" t="e">
-        <v>#DIV/0!</v>
+      <c r="AA48" s="15">
+        <f t="shared" si="9"/>
+        <v>635.66666666666663</v>
       </c>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A49" s="12"/>
-      <c r="B49" s="49"/>
+      <c r="B49" s="45"/>
       <c r="C49" s="26">
         <v>160</v>
       </c>
@@ -5921,13 +5934,14 @@
         <f>10 * 60 + 30</f>
         <v>630</v>
       </c>
-      <c r="AA49" s="29" t="e">
-        <v>#DIV/0!</v>
+      <c r="AA49" s="15">
+        <f t="shared" si="9"/>
+        <v>629.33333333333337</v>
       </c>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A50" s="12"/>
-      <c r="B50" s="47"/>
+      <c r="B50" s="43"/>
       <c r="C50" s="30">
         <v>320</v>
       </c>
@@ -5979,12 +5993,13 @@
         <f>10 * 60 + 29</f>
         <v>629</v>
       </c>
-      <c r="AA50" s="28" t="e">
-        <v>#DIV/0!</v>
+      <c r="AA50" s="15">
+        <f t="shared" si="9"/>
+        <v>629</v>
       </c>
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B51" s="35" t="s">
+      <c r="B51" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="26">
@@ -6016,7 +6031,7 @@
       <c r="AA51" s="9"/>
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B52" s="36"/>
+      <c r="B52" s="37"/>
       <c r="C52" s="26">
         <v>40</v>
       </c>
@@ -6046,7 +6061,7 @@
       <c r="AA52" s="3"/>
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B53" s="36"/>
+      <c r="B53" s="37"/>
       <c r="C53" s="26">
         <v>80</v>
       </c>
@@ -6076,7 +6091,7 @@
       <c r="AA53" s="3"/>
     </row>
     <row r="54" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B54" s="37"/>
+      <c r="B54" s="46"/>
       <c r="C54" s="26">
         <v>160</v>
       </c>
@@ -6106,7 +6121,7 @@
       <c r="AA54" s="3"/>
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B55" s="37"/>
+      <c r="B55" s="46"/>
       <c r="C55" s="30">
         <v>320</v>
       </c>
@@ -6136,7 +6151,7 @@
       <c r="AA55" s="3"/>
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B56" s="35" t="s">
+      <c r="B56" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C56" s="26">
@@ -6168,7 +6183,7 @@
       <c r="AA56" s="9"/>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B57" s="36"/>
+      <c r="B57" s="37"/>
       <c r="C57" s="26">
         <v>40</v>
       </c>
@@ -6198,7 +6213,7 @@
       <c r="AA57" s="3"/>
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B58" s="36"/>
+      <c r="B58" s="37"/>
       <c r="C58" s="26">
         <v>80</v>
       </c>
@@ -6228,7 +6243,7 @@
       <c r="AA58" s="3"/>
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B59" s="36"/>
+      <c r="B59" s="37"/>
       <c r="C59" s="26">
         <v>160</v>
       </c>
@@ -6289,6 +6304,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="T33:W33"/>
+    <mergeCell ref="L33:O33"/>
+    <mergeCell ref="X33:AA33"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B23:B27"/>
     <mergeCell ref="T34:W34"/>
     <mergeCell ref="X34:AA34"/>
     <mergeCell ref="T6:W6"/>
@@ -6305,21 +6335,6 @@
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="P6:S6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="T33:W33"/>
-    <mergeCell ref="L33:O33"/>
-    <mergeCell ref="X33:AA33"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="P5:S5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6331,7 +6346,7 @@
   <dimension ref="B2:S55"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6357,38 +6372,38 @@
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="34" t="s">
+      <c r="C6" s="48"/>
+      <c r="D6" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34" t="s">
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34" t="s">
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="34"/>
-      <c r="S6" s="34"/>
+      <c r="Q6" s="35"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="35"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="18" t="s">
         <v>0</v>
       </c>
@@ -6439,7 +6454,7 @@
       </c>
     </row>
     <row r="8" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="37" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -6472,7 +6487,7 @@
       <c r="S8" s="3"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="37"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
@@ -6503,7 +6518,7 @@
       <c r="S9" s="3"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="37"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -6534,7 +6549,7 @@
       <c r="S10" s="3"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="37"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
@@ -6565,7 +6580,7 @@
       <c r="S11" s="3"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="39"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
@@ -6596,7 +6611,7 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="36" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -6629,7 +6644,7 @@
       <c r="S13" s="9"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B14" s="37"/>
+      <c r="B14" s="46"/>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
@@ -6660,7 +6675,7 @@
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="37"/>
+      <c r="B15" s="46"/>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
@@ -6691,7 +6706,7 @@
       <c r="S15" s="3"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B16" s="37"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
@@ -6722,7 +6737,7 @@
       <c r="S16" s="3"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B17" s="39"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
@@ -6753,7 +6768,7 @@
       <c r="S17" s="6"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="36" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -6786,7 +6801,7 @@
       <c r="S18" s="9"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B19" s="37"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
@@ -6817,7 +6832,7 @@
       <c r="S19" s="3"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B20" s="37"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
@@ -6848,7 +6863,7 @@
       <c r="S20" s="3"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B21" s="37"/>
+      <c r="B21" s="46"/>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
@@ -6879,7 +6894,7 @@
       <c r="S21" s="3"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B22" s="39"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="4" t="s">
         <v>7</v>
       </c>
@@ -6910,7 +6925,7 @@
       <c r="S22" s="6"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -6943,7 +6958,7 @@
       <c r="S23" s="9"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B24" s="37"/>
+      <c r="B24" s="46"/>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
@@ -6974,7 +6989,7 @@
       <c r="S24" s="3"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B25" s="37"/>
+      <c r="B25" s="46"/>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
@@ -7005,7 +7020,7 @@
       <c r="S25" s="3"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B26" s="37"/>
+      <c r="B26" s="46"/>
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
@@ -7036,7 +7051,7 @@
       <c r="S26" s="3"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B27" s="39"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="4" t="s">
         <v>7</v>
       </c>
@@ -7067,7 +7082,7 @@
       <c r="S27" s="6"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -7100,7 +7115,7 @@
       <c r="S28" s="9"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B29" s="36"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
@@ -7131,7 +7146,7 @@
       <c r="S29" s="3"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B30" s="36"/>
+      <c r="B30" s="37"/>
       <c r="C30" s="1" t="s">
         <v>5</v>
       </c>
@@ -7162,7 +7177,7 @@
       <c r="S30" s="3"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B31" s="36"/>
+      <c r="B31" s="37"/>
       <c r="C31" s="1" t="s">
         <v>6</v>
       </c>
@@ -7224,38 +7239,38 @@
       <c r="S32" s="6"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="40"/>
-      <c r="D34" s="34" t="s">
+      <c r="C34" s="48"/>
+      <c r="D34" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34" t="s">
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="34" t="s">
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="M34" s="34"/>
-      <c r="N34" s="34"/>
-      <c r="O34" s="34"/>
-      <c r="P34" s="34" t="s">
+      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="35"/>
+      <c r="P34" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="Q34" s="34"/>
-      <c r="R34" s="34"/>
-      <c r="S34" s="34"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="35"/>
+      <c r="S34" s="35"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
       <c r="D35" s="10" t="s">
         <v>0</v>
       </c>
@@ -7306,7 +7321,7 @@
       </c>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="37" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -7330,7 +7345,7 @@
       <c r="S36" s="3"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B37" s="36"/>
+      <c r="B37" s="37"/>
       <c r="C37" s="1" t="s">
         <v>4</v>
       </c>
@@ -7352,7 +7367,7 @@
       <c r="S37" s="3"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B38" s="37"/>
+      <c r="B38" s="46"/>
       <c r="C38" s="1" t="s">
         <v>5</v>
       </c>
@@ -7374,7 +7389,7 @@
       <c r="S38" s="3"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B39" s="37"/>
+      <c r="B39" s="46"/>
       <c r="C39" s="4" t="s">
         <v>6</v>
       </c>
@@ -7396,7 +7411,7 @@
       <c r="S39" s="3"/>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="36" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -7420,7 +7435,7 @@
       <c r="S40" s="9"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B41" s="36"/>
+      <c r="B41" s="37"/>
       <c r="C41" s="1" t="s">
         <v>4</v>
       </c>
@@ -7442,7 +7457,7 @@
       <c r="S41" s="3"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B42" s="37"/>
+      <c r="B42" s="46"/>
       <c r="C42" s="1" t="s">
         <v>5</v>
       </c>
@@ -7464,7 +7479,7 @@
       <c r="S42" s="3"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B43" s="37"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="4" t="s">
         <v>6</v>
       </c>
@@ -7486,7 +7501,7 @@
       <c r="S43" s="3"/>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="36" t="s">
         <v>10</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -7510,7 +7525,7 @@
       <c r="S44" s="9"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B45" s="36"/>
+      <c r="B45" s="37"/>
       <c r="C45" s="1" t="s">
         <v>4</v>
       </c>
@@ -7532,7 +7547,7 @@
       <c r="S45" s="3"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B46" s="37"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="1" t="s">
         <v>5</v>
       </c>
@@ -7554,7 +7569,7 @@
       <c r="S46" s="3"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B47" s="37"/>
+      <c r="B47" s="46"/>
       <c r="C47" s="4" t="s">
         <v>6</v>
       </c>
@@ -7576,7 +7591,7 @@
       <c r="S47" s="3"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B48" s="35" t="s">
+      <c r="B48" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -7600,7 +7615,7 @@
       <c r="S48" s="9"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B49" s="36"/>
+      <c r="B49" s="37"/>
       <c r="C49" s="1" t="s">
         <v>4</v>
       </c>
@@ -7622,7 +7637,7 @@
       <c r="S49" s="3"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B50" s="37"/>
+      <c r="B50" s="46"/>
       <c r="C50" s="1" t="s">
         <v>5</v>
       </c>
@@ -7644,7 +7659,7 @@
       <c r="S50" s="3"/>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B51" s="37"/>
+      <c r="B51" s="46"/>
       <c r="C51" s="4" t="s">
         <v>6</v>
       </c>
@@ -7666,7 +7681,7 @@
       <c r="S51" s="3"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B52" s="35" t="s">
+      <c r="B52" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C52" s="7" t="s">
@@ -7690,7 +7705,7 @@
       <c r="S52" s="9"/>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B53" s="36"/>
+      <c r="B53" s="37"/>
       <c r="C53" s="1" t="s">
         <v>4</v>
       </c>
@@ -7712,7 +7727,7 @@
       <c r="S53" s="3"/>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B54" s="36"/>
+      <c r="B54" s="37"/>
       <c r="C54" s="1" t="s">
         <v>5</v>
       </c>
@@ -7757,26 +7772,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="P34:S34"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="B8:B12"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="B23:B27"/>
     <mergeCell ref="B28:B32"/>
     <mergeCell ref="B6:C7"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="L34:O34"/>
-    <mergeCell ref="P34:S34"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="B52:B55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Upload revied documents"
This reverts commit c57eb58395073df60e0f3da3ca1132959a6afba0.
</commit_message>
<xml_diff>
--- a/doc/MR_RunningTime.xlsx
+++ b/doc/MR_RunningTime.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18500" yWindow="6820" windowWidth="17680" windowHeight="10020" tabRatio="500"/>
+    <workbookView xWindow="840" yWindow="460" windowWidth="27960" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="1.NumericalSummarization" sheetId="1" r:id="rId1"/>
@@ -481,7 +481,7 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -493,23 +493,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -531,6 +516,21 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -665,7 +665,7 @@
                   <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.33333333333328</c:v>
+                  <c:v>23.33333333333329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -759,10 +759,10 @@
                   <c:v>64.66666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48.66666666666658</c:v>
+                  <c:v>48.66666666666659</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.66666666666658</c:v>
+                  <c:v>37.66666666666659</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -859,7 +859,7 @@
                   <c:v>39.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.66666666666658</c:v>
+                  <c:v>32.66666666666659</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -945,11 +945,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2106700592"/>
-        <c:axId val="2109997312"/>
+        <c:axId val="-2128930544"/>
+        <c:axId val="2138113680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2106700592"/>
+        <c:axId val="-2128930544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -992,7 +992,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109997312"/>
+        <c:crossAx val="2138113680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1000,7 +1000,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109997312"/>
+        <c:axId val="2138113680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180.0"/>
@@ -1111,7 +1111,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2106700592"/>
+        <c:crossAx val="-2128930544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="60.0"/>
@@ -1491,11 +1491,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2108521504"/>
-        <c:axId val="2108524848"/>
+        <c:axId val="-2127045488"/>
+        <c:axId val="-2128850432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2108521504"/>
+        <c:axId val="-2127045488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1538,7 +1538,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108524848"/>
+        <c:crossAx val="-2128850432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1546,7 +1546,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108524848"/>
+        <c:axId val="-2128850432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600.0"/>
@@ -1657,7 +1657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108521504"/>
+        <c:crossAx val="-2127045488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100.0"/>
@@ -3181,8 +3181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AD60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I11" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3210,36 +3210,36 @@
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C5" s="12"/>
-      <c r="L5" s="34" t="s">
+      <c r="L5" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34" t="s">
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="34" t="s">
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="50"/>
+      <c r="T5" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="U5" s="34"/>
-      <c r="V5" s="34"/>
-      <c r="W5" s="34"/>
-      <c r="X5" s="34" t="s">
+      <c r="U5" s="50"/>
+      <c r="V5" s="50"/>
+      <c r="W5" s="50"/>
+      <c r="X5" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="Y5" s="34"/>
-      <c r="Z5" s="34"/>
-      <c r="AA5" s="34"/>
+      <c r="Y5" s="50"/>
+      <c r="Z5" s="50"/>
+      <c r="AA5" s="50"/>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="41"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="35" t="s">
         <v>14</v>
       </c>
@@ -3278,8 +3278,8 @@
       <c r="AA6" s="35"/>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="14" t="s">
         <v>0</v>
       </c>
@@ -3436,7 +3436,7 @@
       </c>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B9" s="38"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
@@ -3516,7 +3516,7 @@
       </c>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B10" s="38"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -3596,7 +3596,7 @@
       </c>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B11" s="38"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
@@ -3676,7 +3676,7 @@
       </c>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B12" s="40"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
@@ -3776,20 +3776,20 @@
         <v>199</v>
       </c>
       <c r="L13" s="23">
-        <f>26 * 60 + 35</f>
-        <v>1595</v>
+        <f>10 * 60 + 14</f>
+        <v>614</v>
       </c>
       <c r="M13" s="23">
-        <f>26 * 60 + 42</f>
-        <v>1602</v>
+        <f xml:space="preserve"> 10 * 60 + 8</f>
+        <v>608</v>
       </c>
       <c r="N13" s="23">
-        <f>27 * 60 + 25</f>
-        <v>1645</v>
+        <f>10*60 +9</f>
+        <v>609</v>
       </c>
       <c r="O13" s="15">
         <f t="shared" si="2"/>
-        <v>1614</v>
+        <v>610.33333333333337</v>
       </c>
       <c r="P13" s="8">
         <v>220</v>
@@ -3838,7 +3838,7 @@
       </c>
     </row>
     <row r="14" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B14" s="38"/>
+      <c r="B14" s="46"/>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
@@ -3918,7 +3918,7 @@
       </c>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B15" s="38"/>
+      <c r="B15" s="46"/>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
@@ -3998,7 +3998,7 @@
       </c>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="38"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
@@ -4078,7 +4078,7 @@
       </c>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B17" s="40"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
@@ -4176,20 +4176,20 @@
         <v>0</v>
       </c>
       <c r="L18" s="23">
-        <f>27 * 60 + 22</f>
-        <v>1642</v>
+        <f xml:space="preserve"> 10 * 60 + 34</f>
+        <v>634</v>
       </c>
       <c r="M18" s="23">
-        <f>26 * 60 + 16</f>
-        <v>1576</v>
+        <f>10 * 60 + 13</f>
+        <v>613</v>
       </c>
       <c r="N18" s="23">
-        <f>26 * 60 + 16</f>
-        <v>1576</v>
+        <f>10*60+13</f>
+        <v>613</v>
       </c>
       <c r="O18" s="15">
         <f t="shared" si="2"/>
-        <v>1598</v>
+        <v>620</v>
       </c>
       <c r="P18" s="8">
         <v>156</v>
@@ -4238,7 +4238,7 @@
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B19" s="38"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
@@ -4316,7 +4316,7 @@
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B20" s="38"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
@@ -4394,7 +4394,7 @@
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B21" s="38"/>
+      <c r="B21" s="46"/>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
@@ -4472,7 +4472,7 @@
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B22" s="40"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="4" t="s">
         <v>7</v>
       </c>
@@ -4594,7 +4594,7 @@
       <c r="AA23" s="15"/>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B24" s="38"/>
+      <c r="B24" s="46"/>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
@@ -4638,7 +4638,7 @@
       <c r="AA24" s="15"/>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B25" s="38"/>
+      <c r="B25" s="46"/>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
@@ -4682,7 +4682,7 @@
       <c r="AA25" s="15"/>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B26" s="38"/>
+      <c r="B26" s="46"/>
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
@@ -4726,7 +4726,7 @@
       <c r="AA26" s="15"/>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B27" s="40"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="4" t="s">
         <v>7</v>
       </c>
@@ -4928,7 +4928,7 @@
       <c r="AA31" s="15"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B32" s="39"/>
+      <c r="B32" s="38"/>
       <c r="C32" s="4" t="s">
         <v>7</v>
       </c>
@@ -4966,72 +4966,72 @@
       <c r="AA32" s="17"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="L33" s="34" t="s">
+      <c r="L33" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="M33" s="34"/>
-      <c r="N33" s="34"/>
-      <c r="O33" s="34"/>
-      <c r="T33" s="34" t="s">
+      <c r="M33" s="50"/>
+      <c r="N33" s="50"/>
+      <c r="O33" s="50"/>
+      <c r="T33" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="U33" s="34"/>
-      <c r="V33" s="34"/>
-      <c r="W33" s="34"/>
-      <c r="X33" s="34" t="s">
+      <c r="U33" s="50"/>
+      <c r="V33" s="50"/>
+      <c r="W33" s="50"/>
+      <c r="X33" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="Y33" s="34"/>
-      <c r="Z33" s="34"/>
-      <c r="AA33" s="34"/>
+      <c r="Y33" s="50"/>
+      <c r="Z33" s="50"/>
+      <c r="AA33" s="50"/>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="12"/>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="44"/>
-      <c r="D34" s="43" t="s">
+      <c r="C34" s="39"/>
+      <c r="D34" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43" t="s">
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43" t="s">
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="M34" s="43"/>
-      <c r="N34" s="43"/>
-      <c r="O34" s="43"/>
+      <c r="M34" s="34"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="34"/>
       <c r="P34" s="35" t="s">
         <v>24</v>
       </c>
       <c r="Q34" s="35"/>
       <c r="R34" s="35"/>
       <c r="S34" s="35"/>
-      <c r="T34" s="43" t="s">
+      <c r="T34" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="U34" s="43"/>
-      <c r="V34" s="43"/>
-      <c r="W34" s="43"/>
-      <c r="X34" s="43" t="s">
+      <c r="U34" s="34"/>
+      <c r="V34" s="34"/>
+      <c r="W34" s="34"/>
+      <c r="X34" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="Y34" s="43"/>
-      <c r="Z34" s="43"/>
-      <c r="AA34" s="43"/>
+      <c r="Y34" s="34"/>
+      <c r="Z34" s="34"/>
+      <c r="AA34" s="34"/>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="12"/>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
       <c r="D35" s="24" t="s">
         <v>0</v>
       </c>
@@ -5107,7 +5107,7 @@
     </row>
     <row r="36" spans="1:30" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="12"/>
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="41" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="26">
@@ -5171,7 +5171,7 @@
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="12"/>
-      <c r="B37" s="47"/>
+      <c r="B37" s="42"/>
       <c r="C37" s="26">
         <v>40</v>
       </c>
@@ -5230,7 +5230,7 @@
     </row>
     <row r="38" spans="1:30" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="12"/>
-      <c r="B38" s="47"/>
+      <c r="B38" s="42"/>
       <c r="C38" s="26">
         <v>80</v>
       </c>
@@ -5289,7 +5289,7 @@
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" s="12"/>
-      <c r="B39" s="47"/>
+      <c r="B39" s="42"/>
       <c r="C39" s="26">
         <v>160</v>
       </c>
@@ -5348,7 +5348,7 @@
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="12"/>
-      <c r="B40" s="48"/>
+      <c r="B40" s="43"/>
       <c r="C40" s="30">
         <v>320</v>
       </c>
@@ -5407,7 +5407,7 @@
     </row>
     <row r="41" spans="1:30" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="12"/>
-      <c r="B41" s="49" t="s">
+      <c r="B41" s="44" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="26">
@@ -5468,7 +5468,7 @@
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="12"/>
-      <c r="B42" s="50"/>
+      <c r="B42" s="45"/>
       <c r="C42" s="26">
         <v>40</v>
       </c>
@@ -5524,7 +5524,7 @@
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="12"/>
-      <c r="B43" s="50"/>
+      <c r="B43" s="45"/>
       <c r="C43" s="26">
         <v>80</v>
       </c>
@@ -5585,7 +5585,7 @@
       <c r="A44" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="50"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="26">
         <v>160</v>
       </c>
@@ -5644,7 +5644,7 @@
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" s="12"/>
-      <c r="B45" s="48"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="30">
         <v>320</v>
       </c>
@@ -5703,7 +5703,7 @@
     </row>
     <row r="46" spans="1:30" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="12"/>
-      <c r="B46" s="49" t="s">
+      <c r="B46" s="44" t="s">
         <v>10</v>
       </c>
       <c r="C46" s="26">
@@ -5764,7 +5764,7 @@
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="12"/>
-      <c r="B47" s="50"/>
+      <c r="B47" s="45"/>
       <c r="C47" s="26">
         <v>40</v>
       </c>
@@ -5823,7 +5823,7 @@
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="12"/>
-      <c r="B48" s="50"/>
+      <c r="B48" s="45"/>
       <c r="C48" s="26">
         <v>80</v>
       </c>
@@ -5882,7 +5882,7 @@
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A49" s="12"/>
-      <c r="B49" s="50"/>
+      <c r="B49" s="45"/>
       <c r="C49" s="26">
         <v>160</v>
       </c>
@@ -5941,7 +5941,7 @@
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A50" s="12"/>
-      <c r="B50" s="48"/>
+      <c r="B50" s="43"/>
       <c r="C50" s="30">
         <v>320</v>
       </c>
@@ -6091,7 +6091,7 @@
       <c r="AA53" s="3"/>
     </row>
     <row r="54" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B54" s="38"/>
+      <c r="B54" s="46"/>
       <c r="C54" s="26">
         <v>160</v>
       </c>
@@ -6121,7 +6121,7 @@
       <c r="AA54" s="3"/>
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B55" s="38"/>
+      <c r="B55" s="46"/>
       <c r="C55" s="30">
         <v>320</v>
       </c>
@@ -6273,7 +6273,7 @@
       <c r="AA59" s="3"/>
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B60" s="39"/>
+      <c r="B60" s="38"/>
       <c r="C60" s="30">
         <v>320</v>
       </c>
@@ -6304,6 +6304,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="T33:W33"/>
+    <mergeCell ref="L33:O33"/>
+    <mergeCell ref="X33:AA33"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B23:B27"/>
     <mergeCell ref="T34:W34"/>
     <mergeCell ref="X34:AA34"/>
     <mergeCell ref="T6:W6"/>
@@ -6320,21 +6335,6 @@
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="P6:S6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="T33:W33"/>
-    <mergeCell ref="L33:O33"/>
-    <mergeCell ref="X33:AA33"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="P5:S5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6345,8 +6345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S55"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6372,10 +6372,10 @@
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="41"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="35" t="s">
         <v>25</v>
       </c>
@@ -6402,8 +6402,8 @@
       <c r="S6" s="35"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="18" t="s">
         <v>0</v>
       </c>
@@ -6487,7 +6487,7 @@
       <c r="S8" s="3"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="38"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
@@ -6518,7 +6518,7 @@
       <c r="S9" s="3"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="38"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -6549,7 +6549,7 @@
       <c r="S10" s="3"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="38"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
@@ -6580,7 +6580,7 @@
       <c r="S11" s="3"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="40"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
@@ -6644,7 +6644,7 @@
       <c r="S13" s="9"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B14" s="38"/>
+      <c r="B14" s="46"/>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
@@ -6675,7 +6675,7 @@
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="38"/>
+      <c r="B15" s="46"/>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
@@ -6706,7 +6706,7 @@
       <c r="S15" s="3"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B16" s="38"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
@@ -6737,7 +6737,7 @@
       <c r="S16" s="3"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B17" s="40"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
@@ -6801,7 +6801,7 @@
       <c r="S18" s="9"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B19" s="38"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
@@ -6832,7 +6832,7 @@
       <c r="S19" s="3"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B20" s="38"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
@@ -6863,7 +6863,7 @@
       <c r="S20" s="3"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B21" s="38"/>
+      <c r="B21" s="46"/>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
@@ -6894,7 +6894,7 @@
       <c r="S21" s="3"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B22" s="40"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="4" t="s">
         <v>7</v>
       </c>
@@ -6958,7 +6958,7 @@
       <c r="S23" s="9"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B24" s="38"/>
+      <c r="B24" s="46"/>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
@@ -6989,7 +6989,7 @@
       <c r="S24" s="3"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B25" s="38"/>
+      <c r="B25" s="46"/>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
@@ -7020,7 +7020,7 @@
       <c r="S25" s="3"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B26" s="38"/>
+      <c r="B26" s="46"/>
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
@@ -7051,7 +7051,7 @@
       <c r="S26" s="3"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B27" s="40"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="4" t="s">
         <v>7</v>
       </c>
@@ -7208,7 +7208,7 @@
       <c r="S31" s="3"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B32" s="39"/>
+      <c r="B32" s="38"/>
       <c r="C32" s="4" t="s">
         <v>7</v>
       </c>
@@ -7239,10 +7239,10 @@
       <c r="S32" s="6"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B34" s="41" t="s">
+      <c r="B34" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="41"/>
+      <c r="C34" s="48"/>
       <c r="D34" s="35" t="s">
         <v>25</v>
       </c>
@@ -7269,8 +7269,8 @@
       <c r="S34" s="35"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
       <c r="D35" s="10" t="s">
         <v>0</v>
       </c>
@@ -7367,7 +7367,7 @@
       <c r="S37" s="3"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B38" s="38"/>
+      <c r="B38" s="46"/>
       <c r="C38" s="1" t="s">
         <v>5</v>
       </c>
@@ -7389,7 +7389,7 @@
       <c r="S38" s="3"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B39" s="38"/>
+      <c r="B39" s="46"/>
       <c r="C39" s="4" t="s">
         <v>6</v>
       </c>
@@ -7457,7 +7457,7 @@
       <c r="S41" s="3"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B42" s="38"/>
+      <c r="B42" s="46"/>
       <c r="C42" s="1" t="s">
         <v>5</v>
       </c>
@@ -7479,7 +7479,7 @@
       <c r="S42" s="3"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B43" s="38"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="4" t="s">
         <v>6</v>
       </c>
@@ -7547,7 +7547,7 @@
       <c r="S45" s="3"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B46" s="38"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="1" t="s">
         <v>5</v>
       </c>
@@ -7569,7 +7569,7 @@
       <c r="S46" s="3"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B47" s="38"/>
+      <c r="B47" s="46"/>
       <c r="C47" s="4" t="s">
         <v>6</v>
       </c>
@@ -7637,7 +7637,7 @@
       <c r="S49" s="3"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B50" s="38"/>
+      <c r="B50" s="46"/>
       <c r="C50" s="1" t="s">
         <v>5</v>
       </c>
@@ -7659,7 +7659,7 @@
       <c r="S50" s="3"/>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B51" s="38"/>
+      <c r="B51" s="46"/>
       <c r="C51" s="4" t="s">
         <v>6</v>
       </c>
@@ -7749,7 +7749,7 @@
       <c r="S54" s="3"/>
     </row>
     <row r="55" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B55" s="39"/>
+      <c r="B55" s="38"/>
       <c r="C55" s="4" t="s">
         <v>6</v>
       </c>
@@ -7772,26 +7772,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="P34:S34"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="B8:B12"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="B23:B27"/>
     <mergeCell ref="B28:B32"/>
     <mergeCell ref="B6:C7"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="L34:O34"/>
-    <mergeCell ref="P34:S34"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="B52:B55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>